<commit_message>
Complete data input spreadsheet
</commit_message>
<xml_diff>
--- a/modules/input_3.xlsx
+++ b/modules/input_3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7890"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7890" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="population_size" sheetId="8" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="TB prevalence" sheetId="4" r:id="rId5"/>
     <sheet name="TB incidence" sheetId="5" r:id="rId6"/>
     <sheet name="comorbidity" sheetId="6" r:id="rId7"/>
+    <sheet name="testing_and_treatment" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="105">
   <si>
     <t>best</t>
   </si>
@@ -267,6 +268,75 @@
   <si>
     <t>Population size</t>
   </si>
+  <si>
+    <t>Percentage of population tested for active TB in the last 12 months</t>
+  </si>
+  <si>
+    <t>Percentage of population tested for latent TB in the last 12 months</t>
+  </si>
+  <si>
+    <t>Percentage of population tested for TB susceptibility in the last 12 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of people initiating treatment for active TB each year </t>
+  </si>
+  <si>
+    <t>Number of people successfully completing treatment for active TB each year</t>
+  </si>
+  <si>
+    <t>Number of people initiating treatment for latent TB each year</t>
+  </si>
+  <si>
+    <t>Number of people successfully completing treatment for latent TB each year</t>
+  </si>
+  <si>
+    <t>0-4 years DS-TB regimen</t>
+  </si>
+  <si>
+    <t>0-4 years MDR-TB regimen</t>
+  </si>
+  <si>
+    <t>0-4 years XDR-TB regimen</t>
+  </si>
+  <si>
+    <t>5-14 years DS-TB regimen</t>
+  </si>
+  <si>
+    <t>5-14 years MDR-TB regimen</t>
+  </si>
+  <si>
+    <t>5-14 years XDR-TB regimen</t>
+  </si>
+  <si>
+    <t>15+ years DS-TB regimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15+ years MDR-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15+ years XDR-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-4 years DS-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-4 years MDR-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-4 years XDR-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-14 years DS-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-14 years MDR-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-14 years XDR-TB regimen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15+ years DS-TB regimen </t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +347,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +418,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -469,7 +545,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="664">
+  <cellStyleXfs count="665">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1134,8 +1210,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1300,8 +1377,32 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="664" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="664" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="664" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="664" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="664">
+  <cellStyles count="665">
     <cellStyle name="Comma 2" xfId="5"/>
     <cellStyle name="Comma 2 2" xfId="6"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -1964,6 +2065,7 @@
     <cellStyle name="Normal 8 2" xfId="660"/>
     <cellStyle name="Normal 9" xfId="661"/>
     <cellStyle name="Normal 9 2" xfId="2"/>
+    <cellStyle name="Percent" xfId="664" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="662"/>
     <cellStyle name="Percent 2 2" xfId="663"/>
   </cellStyles>
@@ -2267,7 +2369,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
@@ -6917,7 +7019,7 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13704,4 +13806,2806 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr published="0"/>
+  <dimension ref="A1:U69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49:S51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.28515625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="20" width="8.5703125" style="40"/>
+    <col min="21" max="21" width="14.28515625" style="40" customWidth="1"/>
+    <col min="22" max="16384" width="8.5703125" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="46"/>
+      <c r="C1" s="11">
+        <v>2000</v>
+      </c>
+      <c r="D1" s="11">
+        <v>2001</v>
+      </c>
+      <c r="E1" s="11">
+        <v>2002</v>
+      </c>
+      <c r="F1" s="11">
+        <v>2003</v>
+      </c>
+      <c r="G1" s="11">
+        <v>2004</v>
+      </c>
+      <c r="H1" s="11">
+        <v>2005</v>
+      </c>
+      <c r="I1" s="11">
+        <v>2006</v>
+      </c>
+      <c r="J1" s="11">
+        <v>2007</v>
+      </c>
+      <c r="K1" s="11">
+        <v>2008</v>
+      </c>
+      <c r="L1" s="11">
+        <v>2009</v>
+      </c>
+      <c r="M1" s="11">
+        <v>2010</v>
+      </c>
+      <c r="N1" s="11">
+        <v>2011</v>
+      </c>
+      <c r="O1" s="11">
+        <v>2012</v>
+      </c>
+      <c r="P1" s="11">
+        <v>2013</v>
+      </c>
+      <c r="Q1" s="11">
+        <v>2014</v>
+      </c>
+      <c r="R1" s="11">
+        <v>2015</v>
+      </c>
+      <c r="S1" s="11">
+        <v>2016</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="69">
+        <v>0.12</v>
+      </c>
+      <c r="D3" s="69">
+        <v>0.13</v>
+      </c>
+      <c r="E3" s="69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F3" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="G3" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="H3" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="I3" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="J3" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="K3" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="M3" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="N3" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="O3" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="P3" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="Q3" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="R3" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="S3" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="27"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="E4" s="69">
+        <v>0.12</v>
+      </c>
+      <c r="F4" s="69">
+        <v>0.13</v>
+      </c>
+      <c r="G4" s="69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H4" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="I4" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="J4" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="K4" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="L4" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="M4" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="N4" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="O4" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="P4" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="Q4" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="R4" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="S4" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" s="27"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="69">
+        <v>0.08</v>
+      </c>
+      <c r="D5" s="69">
+        <v>0.09</v>
+      </c>
+      <c r="E5" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="G5" s="69">
+        <v>0.12</v>
+      </c>
+      <c r="H5" s="69">
+        <v>0.13</v>
+      </c>
+      <c r="I5" s="69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J5" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="K5" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="L5" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="M5" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="N5" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="O5" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="P5" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="Q5" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="R5" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="S5" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" s="14"/>
+    </row>
+    <row r="6" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="40"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70"/>
+      <c r="S7" s="70"/>
+      <c r="T7" s="21"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="D8" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="E8" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="F8" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="G8" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="I8" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="J8" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K8" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L8" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="M8" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="N8" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="O8" s="69">
+        <v>0.33</v>
+      </c>
+      <c r="P8" s="69">
+        <v>0.34</v>
+      </c>
+      <c r="Q8" s="69">
+        <v>0.35</v>
+      </c>
+      <c r="R8" s="69">
+        <v>0.36</v>
+      </c>
+      <c r="S8" s="69">
+        <v>0.37</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U8" s="27"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="D9" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="E9" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="G9" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="H9" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="I9" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="J9" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="K9" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="L9" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="M9" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N9" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O9" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="P9" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="Q9" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="R9" s="69">
+        <v>0.33</v>
+      </c>
+      <c r="S9" s="69">
+        <v>0.34</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U9" s="27"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="D10" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="E10" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="F10" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="G10" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="I10" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="J10" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="K10" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="L10" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="M10" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="N10" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="O10" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P10" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q10" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="R10" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="S10" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U10" s="27"/>
+    </row>
+    <row r="11" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="64"/>
+    </row>
+    <row r="12" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="65"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="64"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="E13" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="F13" s="69">
+        <v>0.33</v>
+      </c>
+      <c r="G13" s="69">
+        <v>0.34</v>
+      </c>
+      <c r="H13" s="69">
+        <v>0.35</v>
+      </c>
+      <c r="I13" s="69">
+        <v>0.36</v>
+      </c>
+      <c r="J13" s="69">
+        <v>0.37</v>
+      </c>
+      <c r="K13" s="69">
+        <v>0.38</v>
+      </c>
+      <c r="L13" s="69">
+        <v>0.39</v>
+      </c>
+      <c r="M13" s="69">
+        <v>0.4</v>
+      </c>
+      <c r="N13" s="69">
+        <v>0.41</v>
+      </c>
+      <c r="O13" s="69">
+        <v>0.42</v>
+      </c>
+      <c r="P13" s="69">
+        <v>0.43</v>
+      </c>
+      <c r="Q13" s="69">
+        <v>0.44</v>
+      </c>
+      <c r="R13" s="69">
+        <v>0.45</v>
+      </c>
+      <c r="S13" s="69">
+        <v>0.46</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U13" s="27"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="69">
+        <v>0.45</v>
+      </c>
+      <c r="D14" s="69">
+        <v>0.46</v>
+      </c>
+      <c r="E14" s="69">
+        <v>0.47</v>
+      </c>
+      <c r="F14" s="69">
+        <v>0.48</v>
+      </c>
+      <c r="G14" s="69">
+        <v>0.49</v>
+      </c>
+      <c r="H14" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="69">
+        <v>0.51</v>
+      </c>
+      <c r="J14" s="69">
+        <v>0.52</v>
+      </c>
+      <c r="K14" s="69">
+        <v>0.53</v>
+      </c>
+      <c r="L14" s="69">
+        <v>0.54</v>
+      </c>
+      <c r="M14" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N14" s="69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O14" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="P14" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q14" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="R14" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="S14" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U14" s="27"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="D15" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="E15" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="F15" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="G15" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="I15" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="J15" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="K15" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="L15" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="M15" s="69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N15" s="69">
+        <v>0.13</v>
+      </c>
+      <c r="O15" s="69">
+        <v>0.12</v>
+      </c>
+      <c r="P15" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="Q15" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="R15" s="69">
+        <v>0.09</v>
+      </c>
+      <c r="S15" s="69">
+        <v>0.08</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U15" s="66"/>
+    </row>
+    <row r="16" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="64"/>
+    </row>
+    <row r="17" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="64"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="69">
+        <v>0.67</v>
+      </c>
+      <c r="D18" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="E18" s="69">
+        <v>0.69</v>
+      </c>
+      <c r="F18" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="G18" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="H18" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="I18" s="69">
+        <v>0.73</v>
+      </c>
+      <c r="J18" s="69">
+        <v>0.74</v>
+      </c>
+      <c r="K18" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="L18" s="69">
+        <v>0.76</v>
+      </c>
+      <c r="M18" s="69">
+        <v>0.77</v>
+      </c>
+      <c r="N18" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="O18" s="69">
+        <v>0.79</v>
+      </c>
+      <c r="P18" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="Q18" s="69">
+        <v>0.81</v>
+      </c>
+      <c r="R18" s="69">
+        <v>0.82</v>
+      </c>
+      <c r="S18" s="69">
+        <v>0.83</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U18" s="14"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="69">
+        <v>0.65</v>
+      </c>
+      <c r="D19" s="69">
+        <v>0.66</v>
+      </c>
+      <c r="E19" s="69">
+        <v>0.67</v>
+      </c>
+      <c r="F19" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="G19" s="69">
+        <v>0.69</v>
+      </c>
+      <c r="H19" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="I19" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="J19" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="K19" s="69">
+        <v>0.73</v>
+      </c>
+      <c r="L19" s="69">
+        <v>0.74</v>
+      </c>
+      <c r="M19" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="N19" s="69">
+        <v>0.76</v>
+      </c>
+      <c r="O19" s="69">
+        <v>0.77</v>
+      </c>
+      <c r="P19" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="Q19" s="69">
+        <v>0.79</v>
+      </c>
+      <c r="R19" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="S19" s="69">
+        <v>0.81</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U19" s="14"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="69">
+        <v>0.64</v>
+      </c>
+      <c r="D20" s="69">
+        <v>0.65</v>
+      </c>
+      <c r="E20" s="69">
+        <v>0.66</v>
+      </c>
+      <c r="F20" s="69">
+        <v>0.67</v>
+      </c>
+      <c r="G20" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="H20" s="69">
+        <v>0.69</v>
+      </c>
+      <c r="I20" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="J20" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="K20" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="L20" s="69">
+        <v>0.73</v>
+      </c>
+      <c r="M20" s="69">
+        <v>0.74</v>
+      </c>
+      <c r="N20" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="O20" s="69">
+        <v>0.76</v>
+      </c>
+      <c r="P20" s="69">
+        <v>0.77</v>
+      </c>
+      <c r="Q20" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="R20" s="69">
+        <v>0.79</v>
+      </c>
+      <c r="S20" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U20" s="14"/>
+    </row>
+    <row r="21" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="71"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="64"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="69">
+        <v>0.35</v>
+      </c>
+      <c r="D22" s="69">
+        <v>0.36</v>
+      </c>
+      <c r="E22" s="69">
+        <v>0.37</v>
+      </c>
+      <c r="F22" s="69">
+        <v>0.38</v>
+      </c>
+      <c r="G22" s="69">
+        <v>0.39</v>
+      </c>
+      <c r="H22" s="69">
+        <v>0.4</v>
+      </c>
+      <c r="I22" s="69">
+        <v>0.41</v>
+      </c>
+      <c r="J22" s="69">
+        <v>0.42</v>
+      </c>
+      <c r="K22" s="69">
+        <v>0.43</v>
+      </c>
+      <c r="L22" s="69">
+        <v>0.44</v>
+      </c>
+      <c r="M22" s="69">
+        <v>0.45</v>
+      </c>
+      <c r="N22" s="69">
+        <v>0.46</v>
+      </c>
+      <c r="O22" s="69">
+        <v>0.47</v>
+      </c>
+      <c r="P22" s="69">
+        <v>0.48</v>
+      </c>
+      <c r="Q22" s="69">
+        <v>0.49</v>
+      </c>
+      <c r="R22" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="S22" s="69">
+        <v>0.51</v>
+      </c>
+      <c r="T22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U22" s="14"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="69">
+        <v>0.33</v>
+      </c>
+      <c r="D23" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="E23" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="F23" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H23" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I23" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="J23" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="K23" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="L23" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="M23" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="N23" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="O23" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="P23" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="Q23" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="R23" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="S23" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U23" s="14"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="D24" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="E24" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F24" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G24" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="H24" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="I24" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="J24" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="K24" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="L24" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="M24" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="N24" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="O24" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="P24" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="Q24" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="R24" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="S24" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="T24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U24" s="14"/>
+    </row>
+    <row r="25" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="71"/>
+      <c r="S25" s="71"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="64"/>
+    </row>
+    <row r="26" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="69">
+        <v>0.66</v>
+      </c>
+      <c r="D26" s="69">
+        <v>0.65</v>
+      </c>
+      <c r="E26" s="69">
+        <v>0.64</v>
+      </c>
+      <c r="F26" s="69">
+        <v>0.63</v>
+      </c>
+      <c r="G26" s="69">
+        <v>0.62</v>
+      </c>
+      <c r="H26" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="I26" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="J26" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="K26" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="L26" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M26" s="69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N26" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O26" s="69">
+        <v>0.54</v>
+      </c>
+      <c r="P26" s="69">
+        <v>0.53</v>
+      </c>
+      <c r="Q26" s="69">
+        <v>0.52</v>
+      </c>
+      <c r="R26" s="69">
+        <v>0.51</v>
+      </c>
+      <c r="S26" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="T26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U26" s="14"/>
+    </row>
+    <row r="27" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="69">
+        <v>0.63</v>
+      </c>
+      <c r="D27" s="69">
+        <v>0.62</v>
+      </c>
+      <c r="E27" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="F27" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="G27" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="H27" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I27" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J27" s="69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K27" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L27" s="69">
+        <v>0.54</v>
+      </c>
+      <c r="M27" s="69">
+        <v>0.53</v>
+      </c>
+      <c r="N27" s="69">
+        <v>0.52</v>
+      </c>
+      <c r="O27" s="69">
+        <v>0.51</v>
+      </c>
+      <c r="P27" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="Q27" s="69">
+        <v>0.49</v>
+      </c>
+      <c r="R27" s="69">
+        <v>0.48</v>
+      </c>
+      <c r="S27" s="69">
+        <v>0.47</v>
+      </c>
+      <c r="T27" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U27" s="14"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="D28" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="E28" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="F28" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G28" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H28" s="69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I28" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J28" s="69">
+        <v>0.54</v>
+      </c>
+      <c r="K28" s="69">
+        <v>0.53</v>
+      </c>
+      <c r="L28" s="69">
+        <v>0.52</v>
+      </c>
+      <c r="M28" s="69">
+        <v>0.51</v>
+      </c>
+      <c r="N28" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="O28" s="69">
+        <v>0.49</v>
+      </c>
+      <c r="P28" s="69">
+        <v>0.48</v>
+      </c>
+      <c r="Q28" s="69">
+        <v>0.47</v>
+      </c>
+      <c r="R28" s="69">
+        <v>0.46</v>
+      </c>
+      <c r="S28" s="69">
+        <v>0.45</v>
+      </c>
+      <c r="T28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U28" s="66"/>
+    </row>
+    <row r="29" spans="1:21" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
+      <c r="O29" s="72"/>
+      <c r="P29" s="72"/>
+      <c r="Q29" s="72"/>
+      <c r="R29" s="72"/>
+      <c r="S29" s="72"/>
+      <c r="T29" s="38"/>
+      <c r="U29" s="68"/>
+    </row>
+    <row r="30" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="71"/>
+      <c r="O30" s="71"/>
+      <c r="P30" s="71"/>
+      <c r="Q30" s="71"/>
+      <c r="R30" s="71"/>
+      <c r="S30" s="71"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="64"/>
+    </row>
+    <row r="31" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="D31" s="69">
+        <v>0.69</v>
+      </c>
+      <c r="E31" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="F31" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="G31" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="H31" s="69">
+        <v>0.73</v>
+      </c>
+      <c r="I31" s="69">
+        <v>0.73999999999999899</v>
+      </c>
+      <c r="J31" s="69">
+        <v>0.749999999999999</v>
+      </c>
+      <c r="K31" s="69">
+        <v>0.75999999999999901</v>
+      </c>
+      <c r="L31" s="69">
+        <v>0.76999999999999902</v>
+      </c>
+      <c r="M31" s="69">
+        <v>0.77999999999999903</v>
+      </c>
+      <c r="N31" s="69">
+        <v>0.78999999999999904</v>
+      </c>
+      <c r="O31" s="69">
+        <v>0.79999999999999905</v>
+      </c>
+      <c r="P31" s="69">
+        <v>0.80999999999999905</v>
+      </c>
+      <c r="Q31" s="69">
+        <v>0.81999999999999895</v>
+      </c>
+      <c r="R31" s="69">
+        <v>0.82999999999999796</v>
+      </c>
+      <c r="S31" s="69">
+        <v>0.83999999999999797</v>
+      </c>
+      <c r="T31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U31" s="14"/>
+    </row>
+    <row r="32" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="69">
+        <v>0.66</v>
+      </c>
+      <c r="D32" s="69">
+        <v>0.65</v>
+      </c>
+      <c r="E32" s="69">
+        <v>0.64</v>
+      </c>
+      <c r="F32" s="69">
+        <v>0.63</v>
+      </c>
+      <c r="G32" s="69">
+        <v>0.62</v>
+      </c>
+      <c r="H32" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="I32" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="J32" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="K32" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="L32" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M32" s="69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N32" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O32" s="69">
+        <v>0.54</v>
+      </c>
+      <c r="P32" s="69">
+        <v>0.53</v>
+      </c>
+      <c r="Q32" s="69">
+        <v>0.52</v>
+      </c>
+      <c r="R32" s="69">
+        <v>0.51</v>
+      </c>
+      <c r="S32" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="T32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U32" s="14"/>
+    </row>
+    <row r="33" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="69">
+        <v>0.64</v>
+      </c>
+      <c r="D33" s="69">
+        <v>0.63</v>
+      </c>
+      <c r="E33" s="69">
+        <v>0.62</v>
+      </c>
+      <c r="F33" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="G33" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="H33" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="I33" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J33" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K33" s="69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L33" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M33" s="69">
+        <v>0.54</v>
+      </c>
+      <c r="N33" s="69">
+        <v>0.53</v>
+      </c>
+      <c r="O33" s="69">
+        <v>0.52</v>
+      </c>
+      <c r="P33" s="69">
+        <v>0.51</v>
+      </c>
+      <c r="Q33" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="R33" s="69">
+        <v>0.49</v>
+      </c>
+      <c r="S33" s="69">
+        <v>0.48</v>
+      </c>
+      <c r="T33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U33" s="14"/>
+    </row>
+    <row r="34" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
+      <c r="L34" s="71"/>
+      <c r="M34" s="71"/>
+      <c r="N34" s="71"/>
+      <c r="O34" s="71"/>
+      <c r="P34" s="71"/>
+      <c r="Q34" s="71"/>
+      <c r="R34" s="71"/>
+      <c r="S34" s="71"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="64"/>
+    </row>
+    <row r="35" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="69">
+        <v>0.85</v>
+      </c>
+      <c r="D35" s="69">
+        <v>0.86</v>
+      </c>
+      <c r="E35" s="69">
+        <v>0.87</v>
+      </c>
+      <c r="F35" s="69">
+        <v>0.88</v>
+      </c>
+      <c r="G35" s="69">
+        <v>0.89</v>
+      </c>
+      <c r="H35" s="69">
+        <v>0.9</v>
+      </c>
+      <c r="I35" s="69">
+        <v>0.91</v>
+      </c>
+      <c r="J35" s="69">
+        <v>0.92</v>
+      </c>
+      <c r="K35" s="69">
+        <v>0.93</v>
+      </c>
+      <c r="L35" s="69">
+        <v>0.94</v>
+      </c>
+      <c r="M35" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="N35" s="69">
+        <v>0.96</v>
+      </c>
+      <c r="O35" s="69">
+        <v>0.97</v>
+      </c>
+      <c r="P35" s="69">
+        <v>0.98</v>
+      </c>
+      <c r="Q35" s="69">
+        <v>0.99</v>
+      </c>
+      <c r="R35" s="69">
+        <v>1</v>
+      </c>
+      <c r="S35" s="69">
+        <v>1.01</v>
+      </c>
+      <c r="T35" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U35" s="14"/>
+    </row>
+    <row r="36" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="69">
+        <v>0.84</v>
+      </c>
+      <c r="D36" s="69">
+        <v>0.83</v>
+      </c>
+      <c r="E36" s="69">
+        <v>0.82</v>
+      </c>
+      <c r="F36" s="69">
+        <v>0.81</v>
+      </c>
+      <c r="G36" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="H36" s="69">
+        <v>0.79</v>
+      </c>
+      <c r="I36" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="J36" s="69">
+        <v>0.77</v>
+      </c>
+      <c r="K36" s="69">
+        <v>0.76</v>
+      </c>
+      <c r="L36" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="M36" s="69">
+        <v>0.74</v>
+      </c>
+      <c r="N36" s="69">
+        <v>0.73</v>
+      </c>
+      <c r="O36" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="P36" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="Q36" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="R36" s="69">
+        <v>0.69</v>
+      </c>
+      <c r="S36" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="T36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U36" s="14"/>
+    </row>
+    <row r="37" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="69">
+        <v>0.82</v>
+      </c>
+      <c r="D37" s="69">
+        <v>0.81</v>
+      </c>
+      <c r="E37" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="F37" s="69">
+        <v>0.79</v>
+      </c>
+      <c r="G37" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="H37" s="69">
+        <v>0.77</v>
+      </c>
+      <c r="I37" s="69">
+        <v>0.76000000000000101</v>
+      </c>
+      <c r="J37" s="69">
+        <v>0.750000000000001</v>
+      </c>
+      <c r="K37" s="69">
+        <v>0.74000000000000099</v>
+      </c>
+      <c r="L37" s="69">
+        <v>0.73000000000000098</v>
+      </c>
+      <c r="M37" s="69">
+        <v>0.72000000000000097</v>
+      </c>
+      <c r="N37" s="69">
+        <v>0.71000000000000096</v>
+      </c>
+      <c r="O37" s="69">
+        <v>0.70000000000000095</v>
+      </c>
+      <c r="P37" s="69">
+        <v>0.69000000000000095</v>
+      </c>
+      <c r="Q37" s="69">
+        <v>0.68000000000000105</v>
+      </c>
+      <c r="R37" s="69">
+        <v>0.67000000000000204</v>
+      </c>
+      <c r="S37" s="69">
+        <v>0.66000000000000203</v>
+      </c>
+      <c r="T37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U37" s="14"/>
+    </row>
+    <row r="38" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
+      <c r="N38" s="71"/>
+      <c r="O38" s="71"/>
+      <c r="P38" s="71"/>
+      <c r="Q38" s="71"/>
+      <c r="R38" s="71"/>
+      <c r="S38" s="71"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="64"/>
+    </row>
+    <row r="39" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="69">
+        <v>0.74</v>
+      </c>
+      <c r="D39" s="69">
+        <v>0.73</v>
+      </c>
+      <c r="E39" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="F39" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="G39" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="H39" s="69">
+        <v>0.69</v>
+      </c>
+      <c r="I39" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="J39" s="69">
+        <v>0.67</v>
+      </c>
+      <c r="K39" s="69">
+        <v>0.66</v>
+      </c>
+      <c r="L39" s="69">
+        <v>0.65</v>
+      </c>
+      <c r="M39" s="69">
+        <v>0.64</v>
+      </c>
+      <c r="N39" s="69">
+        <v>0.63</v>
+      </c>
+      <c r="O39" s="69">
+        <v>0.62</v>
+      </c>
+      <c r="P39" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="Q39" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="R39" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="S39" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="T39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U39" s="14"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B40" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="D40" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="E40" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="F40" s="69">
+        <v>0.69</v>
+      </c>
+      <c r="G40" s="69">
+        <v>0.68</v>
+      </c>
+      <c r="H40" s="69">
+        <v>0.67</v>
+      </c>
+      <c r="I40" s="69">
+        <v>0.66</v>
+      </c>
+      <c r="J40" s="69">
+        <v>0.65</v>
+      </c>
+      <c r="K40" s="69">
+        <v>0.64</v>
+      </c>
+      <c r="L40" s="69">
+        <v>0.63</v>
+      </c>
+      <c r="M40" s="69">
+        <v>0.62</v>
+      </c>
+      <c r="N40" s="69">
+        <v>0.61</v>
+      </c>
+      <c r="O40" s="69">
+        <v>0.6</v>
+      </c>
+      <c r="P40" s="69">
+        <v>0.59</v>
+      </c>
+      <c r="Q40" s="69">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="R40" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="S40" s="69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="T40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U40" s="14"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B41" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="69">
+        <v>0.7</v>
+      </c>
+      <c r="D41" s="69">
+        <v>0.71</v>
+      </c>
+      <c r="E41" s="69">
+        <v>0.72</v>
+      </c>
+      <c r="F41" s="69">
+        <v>0.73</v>
+      </c>
+      <c r="G41" s="69">
+        <v>0.74</v>
+      </c>
+      <c r="H41" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="I41" s="69">
+        <v>0.76</v>
+      </c>
+      <c r="J41" s="69">
+        <v>0.77</v>
+      </c>
+      <c r="K41" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="L41" s="69">
+        <v>0.79</v>
+      </c>
+      <c r="M41" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="N41" s="69">
+        <v>0.81</v>
+      </c>
+      <c r="O41" s="69">
+        <v>0.82</v>
+      </c>
+      <c r="P41" s="69">
+        <v>0.83</v>
+      </c>
+      <c r="Q41" s="69">
+        <v>0.84</v>
+      </c>
+      <c r="R41" s="69">
+        <v>0.85</v>
+      </c>
+      <c r="S41" s="69">
+        <v>0.86</v>
+      </c>
+      <c r="T41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U41" s="66"/>
+    </row>
+    <row r="42" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="71"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="71"/>
+      <c r="O42" s="71"/>
+      <c r="P42" s="71"/>
+      <c r="Q42" s="71"/>
+      <c r="R42" s="71"/>
+      <c r="S42" s="71"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="64"/>
+    </row>
+    <row r="43" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="67"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="71"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="71"/>
+      <c r="K43" s="71"/>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
+      <c r="N43" s="71"/>
+      <c r="O43" s="71"/>
+      <c r="P43" s="71"/>
+      <c r="Q43" s="71"/>
+      <c r="R43" s="71"/>
+      <c r="S43" s="71"/>
+      <c r="T43" s="19"/>
+      <c r="U43" s="64"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="69">
+        <v>0.35</v>
+      </c>
+      <c r="D44" s="69">
+        <v>0.34</v>
+      </c>
+      <c r="E44" s="69">
+        <v>0.33</v>
+      </c>
+      <c r="F44" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="G44" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="H44" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="I44" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J44" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K44" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="L44" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="M44" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="N44" s="69">
+        <v>0.24000000000000099</v>
+      </c>
+      <c r="O44" s="69">
+        <v>0.23000000000000101</v>
+      </c>
+      <c r="P44" s="69">
+        <v>0.220000000000001</v>
+      </c>
+      <c r="Q44" s="69">
+        <v>0.21000000000000099</v>
+      </c>
+      <c r="R44" s="69">
+        <v>0.20000000000000101</v>
+      </c>
+      <c r="S44" s="69">
+        <v>0.190000000000001</v>
+      </c>
+      <c r="T44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U44" s="14"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B45" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="69">
+        <v>0.34</v>
+      </c>
+      <c r="D45" s="69">
+        <v>0.33</v>
+      </c>
+      <c r="E45" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="F45" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="G45" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="H45" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I45" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J45" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="K45" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="L45" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="M45" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="N45" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="O45" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="P45" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="Q45" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="R45" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="S45" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="T45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U45" s="14"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B46" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="69">
+        <v>0.32</v>
+      </c>
+      <c r="D46" s="69">
+        <v>0.31</v>
+      </c>
+      <c r="E46" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="F46" s="69">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G46" s="69">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H46" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="I46" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="J46" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="K46" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="L46" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="M46" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="N46" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="O46" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="P46" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="Q46" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="R46" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="S46" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="T46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U46" s="14"/>
+    </row>
+    <row r="47" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="71"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="71"/>
+      <c r="K47" s="71"/>
+      <c r="L47" s="71"/>
+      <c r="M47" s="71"/>
+      <c r="N47" s="71"/>
+      <c r="O47" s="71"/>
+      <c r="P47" s="71"/>
+      <c r="Q47" s="71"/>
+      <c r="R47" s="71"/>
+      <c r="S47" s="71"/>
+      <c r="T47" s="19"/>
+      <c r="U47" s="64"/>
+    </row>
+    <row r="48" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="67"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="71"/>
+      <c r="H48" s="71"/>
+      <c r="I48" s="71"/>
+      <c r="J48" s="71"/>
+      <c r="K48" s="71"/>
+      <c r="L48" s="71"/>
+      <c r="M48" s="71"/>
+      <c r="N48" s="71"/>
+      <c r="O48" s="71"/>
+      <c r="P48" s="71"/>
+      <c r="Q48" s="71"/>
+      <c r="R48" s="71"/>
+      <c r="S48" s="71"/>
+      <c r="T48" s="19"/>
+      <c r="U48" s="64"/>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B49" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="69">
+        <v>0.27</v>
+      </c>
+      <c r="D49" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="E49" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="F49" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="G49" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="H49" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="I49" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="J49" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="K49" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="L49" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="M49" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="N49" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="O49" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="P49" s="69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q49" s="69">
+        <v>0.13</v>
+      </c>
+      <c r="R49" s="69">
+        <v>0.12</v>
+      </c>
+      <c r="S49" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="T49" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U49" s="14"/>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B50" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="69">
+        <v>0.25</v>
+      </c>
+      <c r="D50" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="E50" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="F50" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="G50" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="H50" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="I50" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="J50" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="K50" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="L50" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="M50" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="N50" s="69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O50" s="69">
+        <v>0.13</v>
+      </c>
+      <c r="P50" s="69">
+        <v>0.12</v>
+      </c>
+      <c r="Q50" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="R50" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="S50" s="69">
+        <v>0.09</v>
+      </c>
+      <c r="T50" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U50" s="14"/>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B51" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="D51" s="69">
+        <v>0.21</v>
+      </c>
+      <c r="E51" s="69">
+        <v>0.19</v>
+      </c>
+      <c r="F51" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="G51" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="H51" s="69">
+        <v>0.13</v>
+      </c>
+      <c r="I51" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="J51" s="69">
+        <v>0.09</v>
+      </c>
+      <c r="K51" s="69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L51" s="69">
+        <v>0.05</v>
+      </c>
+      <c r="M51" s="69">
+        <v>0.03</v>
+      </c>
+      <c r="N51" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="O51" s="69">
+        <v>-9.9999999999999794E-3</v>
+      </c>
+      <c r="P51" s="69">
+        <v>-0.03</v>
+      </c>
+      <c r="Q51" s="69">
+        <v>-0.05</v>
+      </c>
+      <c r="R51" s="69">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="S51" s="69">
+        <v>-0.09</v>
+      </c>
+      <c r="T51" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U51" s="14"/>
+    </row>
+    <row r="52" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="19"/>
+      <c r="U52" s="64"/>
+    </row>
+    <row r="53" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="19"/>
+      <c r="U53" s="64"/>
+    </row>
+    <row r="54" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="18"/>
+      <c r="Q54" s="18"/>
+      <c r="R54" s="18"/>
+      <c r="S54" s="18"/>
+      <c r="T54" s="19"/>
+      <c r="U54" s="64"/>
+    </row>
+    <row r="55" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="19"/>
+      <c r="U55" s="64"/>
+    </row>
+    <row r="56" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="19"/>
+      <c r="U56" s="64"/>
+    </row>
+    <row r="57" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="19"/>
+      <c r="U57" s="64"/>
+    </row>
+    <row r="58" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="18"/>
+      <c r="Q58" s="18"/>
+      <c r="R58" s="18"/>
+      <c r="S58" s="18"/>
+      <c r="T58" s="19"/>
+      <c r="U58" s="64"/>
+    </row>
+    <row r="59" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="18"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" s="18"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="19"/>
+      <c r="U59" s="64"/>
+    </row>
+    <row r="60" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="18"/>
+      <c r="Q60" s="18"/>
+      <c r="R60" s="18"/>
+      <c r="S60" s="18"/>
+      <c r="T60" s="19"/>
+      <c r="U60" s="64"/>
+    </row>
+    <row r="61" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+      <c r="T61" s="19"/>
+      <c r="U61" s="64"/>
+    </row>
+    <row r="62" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" s="18"/>
+      <c r="S62" s="18"/>
+      <c r="T62" s="19"/>
+      <c r="U62" s="64"/>
+    </row>
+    <row r="63" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="18"/>
+      <c r="R63" s="18"/>
+      <c r="S63" s="18"/>
+      <c r="T63" s="19"/>
+      <c r="U63" s="64"/>
+    </row>
+    <row r="64" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
+      <c r="P64" s="18"/>
+      <c r="Q64" s="18"/>
+      <c r="R64" s="18"/>
+      <c r="S64" s="18"/>
+      <c r="T64" s="19"/>
+      <c r="U64" s="64"/>
+    </row>
+    <row r="65" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18"/>
+      <c r="S65" s="18"/>
+      <c r="T65" s="19"/>
+      <c r="U65" s="64"/>
+    </row>
+    <row r="66" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="18"/>
+      <c r="Q66" s="18"/>
+      <c r="R66" s="18"/>
+      <c r="S66" s="18"/>
+      <c r="T66" s="19"/>
+      <c r="U66" s="64"/>
+    </row>
+    <row r="67" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="18"/>
+      <c r="R67" s="18"/>
+      <c r="S67" s="18"/>
+      <c r="T67" s="19"/>
+      <c r="U67" s="64"/>
+    </row>
+    <row r="68" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+      <c r="M68" s="18"/>
+      <c r="N68" s="18"/>
+      <c r="O68" s="18"/>
+      <c r="P68" s="18"/>
+      <c r="Q68" s="18"/>
+      <c r="R68" s="18"/>
+      <c r="S68" s="18"/>
+      <c r="T68" s="19"/>
+      <c r="U68" s="64"/>
+    </row>
+    <row r="69" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="18"/>
+      <c r="P69" s="18"/>
+      <c r="Q69" s="18"/>
+      <c r="R69" s="18"/>
+      <c r="S69" s="18"/>
+      <c r="T69" s="19"/>
+      <c r="U69" s="64"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Discuss with Bosco about cost functions
</commit_message>
<xml_diff>
--- a/modules/input_3.xlsx
+++ b/modules/input_3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7890" tabRatio="807" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7890" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="population_size" sheetId="8" r:id="rId1"/>
@@ -456,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -538,17 +538,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="665">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1217,7 +1206,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1366,19 +1355,10 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2379,8 +2359,8 @@
   </sheetPr>
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,7 +2433,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="69" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="35"/>
@@ -2539,7 +2519,9 @@
       <c r="U3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="31"/>
+      <c r="V3" s="31">
+        <v>1500</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
@@ -2602,7 +2584,9 @@
       <c r="U4" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V4" s="31"/>
+      <c r="V4" s="31">
+        <v>1500</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
@@ -2665,29 +2649,31 @@
       <c r="U5" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V5" s="31"/>
+      <c r="V5" s="31">
+        <v>1500</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C6" s="44"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
       <c r="U6" s="43"/>
-      <c r="V6" s="58"/>
+      <c r="V6" s="57"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
@@ -2696,61 +2682,63 @@
       <c r="C7" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="58">
         <v>500</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="58">
         <v>600</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="58">
         <v>700</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="58">
         <v>800</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="58">
         <v>900</v>
       </c>
-      <c r="I7" s="59">
+      <c r="I7" s="58">
         <v>1000</v>
       </c>
-      <c r="J7" s="59">
+      <c r="J7" s="58">
         <v>1100</v>
       </c>
-      <c r="K7" s="59">
+      <c r="K7" s="58">
         <v>1200</v>
       </c>
-      <c r="L7" s="59">
+      <c r="L7" s="58">
         <v>1300</v>
       </c>
-      <c r="M7" s="59">
+      <c r="M7" s="58">
         <v>1400</v>
       </c>
-      <c r="N7" s="59">
+      <c r="N7" s="58">
         <v>1500</v>
       </c>
-      <c r="O7" s="59">
+      <c r="O7" s="58">
         <v>1600</v>
       </c>
-      <c r="P7" s="59">
+      <c r="P7" s="58">
         <v>1700</v>
       </c>
-      <c r="Q7" s="59">
+      <c r="Q7" s="58">
         <v>1800</v>
       </c>
-      <c r="R7" s="59">
+      <c r="R7" s="58">
         <v>1900</v>
       </c>
-      <c r="S7" s="59">
+      <c r="S7" s="58">
         <v>2000</v>
       </c>
-      <c r="T7" s="59">
+      <c r="T7" s="58">
         <v>2100</v>
       </c>
       <c r="U7" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V7" s="60"/>
+      <c r="V7" s="31">
+        <v>1800</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
@@ -2759,61 +2747,63 @@
       <c r="C8" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="58">
         <v>1500</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="58">
         <v>1600</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="58">
         <v>1700</v>
       </c>
-      <c r="G8" s="59">
+      <c r="G8" s="58">
         <v>1800</v>
       </c>
-      <c r="H8" s="59">
+      <c r="H8" s="58">
         <v>1900</v>
       </c>
-      <c r="I8" s="59">
+      <c r="I8" s="58">
         <v>2000</v>
       </c>
-      <c r="J8" s="59">
+      <c r="J8" s="58">
         <v>2100</v>
       </c>
-      <c r="K8" s="59">
+      <c r="K8" s="58">
         <v>2200</v>
       </c>
-      <c r="L8" s="59">
+      <c r="L8" s="58">
         <v>2300</v>
       </c>
-      <c r="M8" s="59">
+      <c r="M8" s="58">
         <v>2400</v>
       </c>
-      <c r="N8" s="59">
+      <c r="N8" s="58">
         <v>2500</v>
       </c>
-      <c r="O8" s="59">
+      <c r="O8" s="58">
         <v>2600</v>
       </c>
-      <c r="P8" s="59">
+      <c r="P8" s="58">
         <v>2700</v>
       </c>
-      <c r="Q8" s="59">
+      <c r="Q8" s="58">
         <v>2800</v>
       </c>
-      <c r="R8" s="59">
+      <c r="R8" s="58">
         <v>2900</v>
       </c>
-      <c r="S8" s="59">
+      <c r="S8" s="58">
         <v>3000</v>
       </c>
-      <c r="T8" s="59">
+      <c r="T8" s="58">
         <v>3100</v>
       </c>
       <c r="U8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V8" s="61"/>
+      <c r="V8" s="31">
+        <v>1800</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -2822,83 +2812,85 @@
       <c r="C9" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="58">
         <v>650</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="58">
         <v>660</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="58">
         <v>670</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="58">
         <v>680</v>
       </c>
-      <c r="H9" s="59">
+      <c r="H9" s="58">
         <v>690</v>
       </c>
-      <c r="I9" s="59">
+      <c r="I9" s="58">
         <v>700</v>
       </c>
-      <c r="J9" s="59">
+      <c r="J9" s="58">
         <v>710</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="58">
         <v>720</v>
       </c>
-      <c r="L9" s="59">
+      <c r="L9" s="58">
         <v>730</v>
       </c>
-      <c r="M9" s="59">
+      <c r="M9" s="58">
         <v>740</v>
       </c>
-      <c r="N9" s="59">
+      <c r="N9" s="58">
         <v>750</v>
       </c>
-      <c r="O9" s="59">
+      <c r="O9" s="58">
         <v>760</v>
       </c>
-      <c r="P9" s="59">
+      <c r="P9" s="58">
         <v>770</v>
       </c>
-      <c r="Q9" s="59">
+      <c r="Q9" s="58">
         <v>780</v>
       </c>
-      <c r="R9" s="59">
+      <c r="R9" s="58">
         <v>790</v>
       </c>
-      <c r="S9" s="59">
+      <c r="S9" s="58">
         <v>800</v>
       </c>
-      <c r="T9" s="59">
+      <c r="T9" s="58">
         <v>810</v>
       </c>
       <c r="U9" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V9" s="57"/>
+      <c r="V9" s="31">
+        <v>1800</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C10" s="44"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="58"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
       <c r="U10" s="43"/>
-      <c r="V10" s="58"/>
+      <c r="V10" s="57"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
@@ -2907,61 +2899,63 @@
       <c r="C11" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="59">
+      <c r="D11" s="58">
         <v>4000</v>
       </c>
-      <c r="E11" s="59">
+      <c r="E11" s="58">
         <v>4500</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="58">
         <v>5000</v>
       </c>
-      <c r="G11" s="59">
+      <c r="G11" s="58">
         <v>5500</v>
       </c>
-      <c r="H11" s="59">
+      <c r="H11" s="58">
         <v>6000</v>
       </c>
-      <c r="I11" s="59">
+      <c r="I11" s="58">
         <v>6500</v>
       </c>
-      <c r="J11" s="59">
+      <c r="J11" s="58">
         <v>7000</v>
       </c>
-      <c r="K11" s="59">
+      <c r="K11" s="58">
         <v>7500</v>
       </c>
-      <c r="L11" s="59">
+      <c r="L11" s="58">
         <v>8000</v>
       </c>
-      <c r="M11" s="59">
+      <c r="M11" s="58">
         <v>8500</v>
       </c>
-      <c r="N11" s="59">
+      <c r="N11" s="58">
         <v>9000</v>
       </c>
-      <c r="O11" s="59">
+      <c r="O11" s="58">
         <v>9500</v>
       </c>
-      <c r="P11" s="59">
+      <c r="P11" s="58">
         <v>10000</v>
       </c>
-      <c r="Q11" s="59">
+      <c r="Q11" s="58">
         <v>10500</v>
       </c>
-      <c r="R11" s="59">
+      <c r="R11" s="58">
         <v>11000</v>
       </c>
-      <c r="S11" s="59">
+      <c r="S11" s="58">
         <v>11500</v>
       </c>
-      <c r="T11" s="59">
+      <c r="T11" s="58">
         <v>12000</v>
       </c>
       <c r="U11" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V11" s="60"/>
+      <c r="V11" s="31">
+        <v>1900</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
@@ -2970,61 +2964,63 @@
       <c r="C12" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="59">
+      <c r="D12" s="58">
         <v>3000</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="58">
         <v>3600</v>
       </c>
-      <c r="F12" s="59">
+      <c r="F12" s="58">
         <v>4200</v>
       </c>
-      <c r="G12" s="59">
+      <c r="G12" s="58">
         <v>4800</v>
       </c>
-      <c r="H12" s="59">
+      <c r="H12" s="58">
         <v>5400</v>
       </c>
-      <c r="I12" s="59">
+      <c r="I12" s="58">
         <v>6000</v>
       </c>
-      <c r="J12" s="59">
+      <c r="J12" s="58">
         <v>6600</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K12" s="58">
         <v>7200</v>
       </c>
-      <c r="L12" s="59">
+      <c r="L12" s="58">
         <v>7800</v>
       </c>
-      <c r="M12" s="59">
+      <c r="M12" s="58">
         <v>8400</v>
       </c>
-      <c r="N12" s="59">
+      <c r="N12" s="58">
         <v>9000</v>
       </c>
-      <c r="O12" s="59">
+      <c r="O12" s="58">
         <v>9600</v>
       </c>
-      <c r="P12" s="59">
+      <c r="P12" s="58">
         <v>10200</v>
       </c>
-      <c r="Q12" s="59">
+      <c r="Q12" s="58">
         <v>10800</v>
       </c>
-      <c r="R12" s="59">
+      <c r="R12" s="58">
         <v>11400</v>
       </c>
-      <c r="S12" s="59">
+      <c r="S12" s="58">
         <v>12000</v>
       </c>
-      <c r="T12" s="59">
+      <c r="T12" s="58">
         <v>12600</v>
       </c>
       <c r="U12" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V12" s="61"/>
+      <c r="V12" s="31">
+        <v>1900</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
@@ -3033,61 +3029,63 @@
       <c r="C13" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="59">
+      <c r="D13" s="58">
         <v>2000</v>
       </c>
-      <c r="E13" s="59">
+      <c r="E13" s="58">
         <v>2100</v>
       </c>
-      <c r="F13" s="59">
+      <c r="F13" s="58">
         <v>2200</v>
       </c>
-      <c r="G13" s="59">
+      <c r="G13" s="58">
         <v>2300</v>
       </c>
-      <c r="H13" s="59">
+      <c r="H13" s="58">
         <v>2400</v>
       </c>
-      <c r="I13" s="59">
+      <c r="I13" s="58">
         <v>2500</v>
       </c>
-      <c r="J13" s="59">
+      <c r="J13" s="58">
         <v>2600</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="58">
         <v>2700</v>
       </c>
-      <c r="L13" s="59">
+      <c r="L13" s="58">
         <v>2800</v>
       </c>
-      <c r="M13" s="59">
+      <c r="M13" s="58">
         <v>2900</v>
       </c>
-      <c r="N13" s="59">
+      <c r="N13" s="58">
         <v>3000</v>
       </c>
-      <c r="O13" s="59">
+      <c r="O13" s="58">
         <v>3100</v>
       </c>
-      <c r="P13" s="59">
+      <c r="P13" s="58">
         <v>3200</v>
       </c>
-      <c r="Q13" s="59">
+      <c r="Q13" s="58">
         <v>3300</v>
       </c>
-      <c r="R13" s="59">
+      <c r="R13" s="58">
         <v>3400</v>
       </c>
-      <c r="S13" s="59">
+      <c r="S13" s="58">
         <v>3500</v>
       </c>
-      <c r="T13" s="59">
+      <c r="T13" s="58">
         <v>3600</v>
       </c>
       <c r="U13" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="V13" s="57"/>
+      <c r="V13" s="31">
+        <v>1900</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3410,7 +3408,9 @@
   </sheetPr>
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:R8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3484,23 +3484,57 @@
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="B2" s="14">
+        <v>10</v>
+      </c>
+      <c r="C2" s="14">
+        <v>11</v>
+      </c>
+      <c r="D2" s="14">
+        <v>12</v>
+      </c>
+      <c r="E2" s="14">
+        <v>13</v>
+      </c>
+      <c r="F2" s="14">
+        <v>14</v>
+      </c>
+      <c r="G2" s="14">
+        <v>15</v>
+      </c>
+      <c r="H2" s="14">
+        <v>16</v>
+      </c>
+      <c r="I2" s="14">
+        <v>17</v>
+      </c>
+      <c r="J2" s="14">
+        <v>18</v>
+      </c>
+      <c r="K2" s="14">
+        <v>19</v>
+      </c>
+      <c r="L2" s="14">
+        <v>20</v>
+      </c>
+      <c r="M2" s="14">
+        <v>21</v>
+      </c>
+      <c r="N2" s="14">
+        <v>22</v>
+      </c>
+      <c r="O2" s="14">
+        <v>23</v>
+      </c>
+      <c r="P2" s="14">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>25</v>
+      </c>
+      <c r="R2" s="14">
+        <v>26</v>
+      </c>
       <c r="S2" s="11" t="s">
         <v>30</v>
       </c>
@@ -3532,23 +3566,57 @@
       <c r="A4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
+      <c r="B4" s="14">
+        <v>10</v>
+      </c>
+      <c r="C4" s="14">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14">
+        <v>12</v>
+      </c>
+      <c r="E4" s="14">
+        <v>13</v>
+      </c>
+      <c r="F4" s="14">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14">
+        <v>15</v>
+      </c>
+      <c r="H4" s="14">
+        <v>16</v>
+      </c>
+      <c r="I4" s="14">
+        <v>17</v>
+      </c>
+      <c r="J4" s="14">
+        <v>18</v>
+      </c>
+      <c r="K4" s="14">
+        <v>19</v>
+      </c>
+      <c r="L4" s="14">
+        <v>20</v>
+      </c>
+      <c r="M4" s="14">
+        <v>21</v>
+      </c>
+      <c r="N4" s="14">
+        <v>22</v>
+      </c>
+      <c r="O4" s="14">
+        <v>23</v>
+      </c>
+      <c r="P4" s="14">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>25</v>
+      </c>
+      <c r="R4" s="14">
+        <v>26</v>
+      </c>
       <c r="S4" s="11" t="s">
         <v>30</v>
       </c>
@@ -3562,23 +3630,57 @@
       <c r="A6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
+      <c r="B6" s="14">
+        <v>10</v>
+      </c>
+      <c r="C6" s="14">
+        <v>11</v>
+      </c>
+      <c r="D6" s="14">
+        <v>12</v>
+      </c>
+      <c r="E6" s="14">
+        <v>13</v>
+      </c>
+      <c r="F6" s="14">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14">
+        <v>15</v>
+      </c>
+      <c r="H6" s="14">
+        <v>16</v>
+      </c>
+      <c r="I6" s="14">
+        <v>17</v>
+      </c>
+      <c r="J6" s="14">
+        <v>18</v>
+      </c>
+      <c r="K6" s="14">
+        <v>19</v>
+      </c>
+      <c r="L6" s="14">
+        <v>20</v>
+      </c>
+      <c r="M6" s="14">
+        <v>21</v>
+      </c>
+      <c r="N6" s="14">
+        <v>22</v>
+      </c>
+      <c r="O6" s="14">
+        <v>23</v>
+      </c>
+      <c r="P6" s="14">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>25</v>
+      </c>
+      <c r="R6" s="14">
+        <v>26</v>
+      </c>
       <c r="S6" s="11" t="s">
         <v>30</v>
       </c>
@@ -3588,23 +3690,57 @@
       <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="B8" s="14">
+        <v>10</v>
+      </c>
+      <c r="C8" s="14">
+        <v>11</v>
+      </c>
+      <c r="D8" s="14">
+        <v>12</v>
+      </c>
+      <c r="E8" s="14">
+        <v>13</v>
+      </c>
+      <c r="F8" s="14">
+        <v>14</v>
+      </c>
+      <c r="G8" s="14">
+        <v>15</v>
+      </c>
+      <c r="H8" s="14">
+        <v>16</v>
+      </c>
+      <c r="I8" s="14">
+        <v>17</v>
+      </c>
+      <c r="J8" s="14">
+        <v>18</v>
+      </c>
+      <c r="K8" s="14">
+        <v>19</v>
+      </c>
+      <c r="L8" s="14">
+        <v>20</v>
+      </c>
+      <c r="M8" s="14">
+        <v>21</v>
+      </c>
+      <c r="N8" s="14">
+        <v>22</v>
+      </c>
+      <c r="O8" s="14">
+        <v>23</v>
+      </c>
+      <c r="P8" s="14">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>25</v>
+      </c>
+      <c r="R8" s="14">
+        <v>26</v>
+      </c>
       <c r="S8" s="11" t="s">
         <v>30</v>
       </c>
@@ -3857,7 +3993,7 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,7 +4008,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="69" t="s">
         <v>104</v>
       </c>
     </row>
@@ -4964,7 +5100,9 @@
   </sheetPr>
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7035,7 +7173,9 @@
   </sheetPr>
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9054,7 +9194,7 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -9150,181 +9290,181 @@
       <c r="B3" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="68">
+      <c r="C3" s="65">
         <v>0.12</v>
       </c>
-      <c r="D3" s="68">
+      <c r="D3" s="65">
         <v>0.13</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F3" s="68">
+      <c r="F3" s="65">
         <v>0.15</v>
       </c>
-      <c r="G3" s="68">
+      <c r="G3" s="65">
         <v>0.16</v>
       </c>
-      <c r="H3" s="68">
+      <c r="H3" s="65">
         <v>0.17</v>
       </c>
-      <c r="I3" s="68">
+      <c r="I3" s="65">
         <v>0.18</v>
       </c>
-      <c r="J3" s="68">
+      <c r="J3" s="65">
         <v>0.19</v>
       </c>
-      <c r="K3" s="68">
+      <c r="K3" s="65">
         <v>0.2</v>
       </c>
-      <c r="L3" s="68">
+      <c r="L3" s="65">
         <v>0.21</v>
       </c>
-      <c r="M3" s="68">
+      <c r="M3" s="65">
         <v>0.22</v>
       </c>
-      <c r="N3" s="68">
+      <c r="N3" s="65">
         <v>0.23</v>
       </c>
-      <c r="O3" s="68">
+      <c r="O3" s="65">
         <v>0.24</v>
       </c>
-      <c r="P3" s="68">
+      <c r="P3" s="65">
         <v>0.25</v>
       </c>
-      <c r="Q3" s="68">
+      <c r="Q3" s="65">
         <v>0.26</v>
       </c>
-      <c r="R3" s="68">
+      <c r="R3" s="65">
         <v>0.27</v>
       </c>
-      <c r="S3" s="68">
+      <c r="S3" s="65">
         <v>0.28000000000000003</v>
       </c>
       <c r="T3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="68"/>
+      <c r="U3" s="65"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="65">
         <v>0.13</v>
       </c>
-      <c r="D4" s="68">
+      <c r="D4" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="65">
         <v>0.15</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="65">
         <v>0.16</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="65">
         <v>0.17</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="65">
         <v>0.18</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="65">
         <v>0.19</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="65">
         <v>0.2</v>
       </c>
-      <c r="K4" s="68">
+      <c r="K4" s="65">
         <v>0.21</v>
       </c>
-      <c r="L4" s="68">
+      <c r="L4" s="65">
         <v>0.22</v>
       </c>
-      <c r="M4" s="68">
+      <c r="M4" s="65">
         <v>0.23</v>
       </c>
-      <c r="N4" s="68">
+      <c r="N4" s="65">
         <v>0.24</v>
       </c>
-      <c r="O4" s="68">
+      <c r="O4" s="65">
         <v>0.25</v>
       </c>
-      <c r="P4" s="68">
+      <c r="P4" s="65">
         <v>0.26</v>
       </c>
-      <c r="Q4" s="68">
+      <c r="Q4" s="65">
         <v>0.27</v>
       </c>
-      <c r="R4" s="68">
+      <c r="R4" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="S4" s="68">
+      <c r="S4" s="65">
         <v>0.28999999999999998</v>
       </c>
       <c r="T4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U4" s="68"/>
+      <c r="U4" s="65"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="68">
+      <c r="C5" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D5" s="68">
+      <c r="D5" s="65">
         <v>0.15</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="65">
         <v>0.16</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="65">
         <v>0.17</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="65">
         <v>0.18</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="65">
         <v>0.19</v>
       </c>
-      <c r="I5" s="68">
+      <c r="I5" s="65">
         <v>0.2</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="65">
         <v>0.21</v>
       </c>
-      <c r="K5" s="68">
+      <c r="K5" s="65">
         <v>0.22</v>
       </c>
-      <c r="L5" s="68">
+      <c r="L5" s="65">
         <v>0.23</v>
       </c>
-      <c r="M5" s="68">
+      <c r="M5" s="65">
         <v>0.24</v>
       </c>
-      <c r="N5" s="68">
+      <c r="N5" s="65">
         <v>0.25</v>
       </c>
-      <c r="O5" s="68">
+      <c r="O5" s="65">
         <v>0.26</v>
       </c>
-      <c r="P5" s="68">
+      <c r="P5" s="65">
         <v>0.27</v>
       </c>
-      <c r="Q5" s="68">
+      <c r="Q5" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R5" s="68">
+      <c r="R5" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S5" s="68">
+      <c r="S5" s="65">
         <v>0.3</v>
       </c>
       <c r="T5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="68"/>
+      <c r="U5" s="65"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
@@ -9335,203 +9475,203 @@
       <c r="B8" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="65">
         <v>0.05</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="65">
         <v>0.06</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="65">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="65">
         <v>0.08</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="65">
         <v>0.09</v>
       </c>
-      <c r="H8" s="68">
+      <c r="H8" s="65">
         <v>0.1</v>
       </c>
-      <c r="I8" s="68">
+      <c r="I8" s="65">
         <v>0.11</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="65">
         <v>0.12</v>
       </c>
-      <c r="K8" s="68">
+      <c r="K8" s="65">
         <v>0.13</v>
       </c>
-      <c r="L8" s="68">
+      <c r="L8" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M8" s="68">
+      <c r="M8" s="65">
         <v>0.15</v>
       </c>
-      <c r="N8" s="68">
+      <c r="N8" s="65">
         <v>0.16</v>
       </c>
-      <c r="O8" s="68">
+      <c r="O8" s="65">
         <v>0.17</v>
       </c>
-      <c r="P8" s="68">
+      <c r="P8" s="65">
         <v>0.18</v>
       </c>
-      <c r="Q8" s="68">
+      <c r="Q8" s="65">
         <v>0.19</v>
       </c>
-      <c r="R8" s="68">
+      <c r="R8" s="65">
         <v>0.2</v>
       </c>
-      <c r="S8" s="68">
+      <c r="S8" s="65">
         <v>0.21</v>
       </c>
       <c r="T8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U8" s="68"/>
+      <c r="U8" s="65"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="65">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="65">
         <v>0.08</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="65">
         <v>0.09</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="65">
         <v>0.1</v>
       </c>
-      <c r="G9" s="68">
+      <c r="G9" s="65">
         <v>0.11</v>
       </c>
-      <c r="H9" s="68">
+      <c r="H9" s="65">
         <v>0.12</v>
       </c>
-      <c r="I9" s="68">
+      <c r="I9" s="65">
         <v>0.13</v>
       </c>
-      <c r="J9" s="68">
+      <c r="J9" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K9" s="68">
+      <c r="K9" s="65">
         <v>0.15</v>
       </c>
-      <c r="L9" s="68">
+      <c r="L9" s="65">
         <v>0.16</v>
       </c>
-      <c r="M9" s="68">
+      <c r="M9" s="65">
         <v>0.17</v>
       </c>
-      <c r="N9" s="68">
+      <c r="N9" s="65">
         <v>0.18</v>
       </c>
-      <c r="O9" s="68">
+      <c r="O9" s="65">
         <v>0.19</v>
       </c>
-      <c r="P9" s="68">
+      <c r="P9" s="65">
         <v>0.2</v>
       </c>
-      <c r="Q9" s="68">
+      <c r="Q9" s="65">
         <v>0.21</v>
       </c>
-      <c r="R9" s="68">
+      <c r="R9" s="65">
         <v>0.22</v>
       </c>
-      <c r="S9" s="68">
+      <c r="S9" s="65">
         <v>0.23</v>
       </c>
       <c r="T9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U9" s="68"/>
+      <c r="U9" s="65"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="65">
         <v>0.09</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="65">
         <v>0.11</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="65">
         <v>0.13</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="65">
         <v>0.15</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="65">
         <v>0.17</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="65">
         <v>0.19</v>
       </c>
-      <c r="I10" s="68">
+      <c r="I10" s="65">
         <v>0.21</v>
       </c>
-      <c r="J10" s="68">
+      <c r="J10" s="65">
         <v>0.23</v>
       </c>
-      <c r="K10" s="68">
+      <c r="K10" s="65">
         <v>0.25</v>
       </c>
-      <c r="L10" s="68">
+      <c r="L10" s="65">
         <v>0.27</v>
       </c>
-      <c r="M10" s="68">
+      <c r="M10" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="N10" s="68">
+      <c r="N10" s="65">
         <v>0.31</v>
       </c>
-      <c r="O10" s="68">
+      <c r="O10" s="65">
         <v>0.33</v>
       </c>
-      <c r="P10" s="68">
+      <c r="P10" s="65">
         <v>0.35</v>
       </c>
-      <c r="Q10" s="68">
+      <c r="Q10" s="65">
         <v>0.37</v>
       </c>
-      <c r="R10" s="68">
+      <c r="R10" s="65">
         <v>0.39</v>
       </c>
-      <c r="S10" s="68">
+      <c r="S10" s="65">
         <v>0.41</v>
       </c>
       <c r="T10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U10" s="68"/>
+      <c r="U10" s="65"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="23"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="73"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="70"/>
+      <c r="P11" s="70"/>
+      <c r="Q11" s="70"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
       <c r="T11" s="11"/>
-      <c r="U11" s="73"/>
+      <c r="U11" s="70"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -14390,7 +14530,7 @@
   </sheetPr>
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -14469,55 +14609,55 @@
       <c r="B3" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="68">
+      <c r="C3" s="65">
         <v>0.12</v>
       </c>
-      <c r="D3" s="68">
+      <c r="D3" s="65">
         <v>0.13</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F3" s="68">
+      <c r="F3" s="65">
         <v>0.15</v>
       </c>
-      <c r="G3" s="68">
+      <c r="G3" s="65">
         <v>0.16</v>
       </c>
-      <c r="H3" s="68">
+      <c r="H3" s="65">
         <v>0.17</v>
       </c>
-      <c r="I3" s="68">
+      <c r="I3" s="65">
         <v>0.18</v>
       </c>
-      <c r="J3" s="68">
+      <c r="J3" s="65">
         <v>0.19</v>
       </c>
-      <c r="K3" s="68">
+      <c r="K3" s="65">
         <v>0.2</v>
       </c>
-      <c r="L3" s="68">
+      <c r="L3" s="65">
         <v>0.21</v>
       </c>
-      <c r="M3" s="68">
+      <c r="M3" s="65">
         <v>0.22</v>
       </c>
-      <c r="N3" s="68">
+      <c r="N3" s="65">
         <v>0.23</v>
       </c>
-      <c r="O3" s="68">
+      <c r="O3" s="65">
         <v>0.24</v>
       </c>
-      <c r="P3" s="68">
+      <c r="P3" s="65">
         <v>0.25</v>
       </c>
-      <c r="Q3" s="68">
+      <c r="Q3" s="65">
         <v>0.26</v>
       </c>
-      <c r="R3" s="68">
+      <c r="R3" s="65">
         <v>0.27</v>
       </c>
-      <c r="S3" s="68">
+      <c r="S3" s="65">
         <v>0.28000000000000003</v>
       </c>
       <c r="T3" s="11" t="s">
@@ -14529,55 +14669,55 @@
       <c r="B4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="65">
         <v>0.1</v>
       </c>
-      <c r="D4" s="68">
+      <c r="D4" s="65">
         <v>0.11</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="65">
         <v>0.12</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="65">
         <v>0.13</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="65">
         <v>0.15</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="65">
         <v>0.16</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="65">
         <v>0.17</v>
       </c>
-      <c r="K4" s="68">
+      <c r="K4" s="65">
         <v>0.18</v>
       </c>
-      <c r="L4" s="68">
+      <c r="L4" s="65">
         <v>0.19</v>
       </c>
-      <c r="M4" s="68">
+      <c r="M4" s="65">
         <v>0.2</v>
       </c>
-      <c r="N4" s="68">
+      <c r="N4" s="65">
         <v>0.21</v>
       </c>
-      <c r="O4" s="68">
+      <c r="O4" s="65">
         <v>0.22</v>
       </c>
-      <c r="P4" s="68">
+      <c r="P4" s="65">
         <v>0.23</v>
       </c>
-      <c r="Q4" s="68">
+      <c r="Q4" s="65">
         <v>0.24</v>
       </c>
-      <c r="R4" s="68">
+      <c r="R4" s="65">
         <v>0.25</v>
       </c>
-      <c r="S4" s="68">
+      <c r="S4" s="65">
         <v>0.26</v>
       </c>
       <c r="T4" s="11" t="s">
@@ -14589,55 +14729,55 @@
       <c r="B5" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="68">
+      <c r="C5" s="65">
         <v>0.08</v>
       </c>
-      <c r="D5" s="68">
+      <c r="D5" s="65">
         <v>0.09</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="65">
         <v>0.1</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="65">
         <v>0.11</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="65">
         <v>0.12</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="65">
         <v>0.13</v>
       </c>
-      <c r="I5" s="68">
+      <c r="I5" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="65">
         <v>0.15</v>
       </c>
-      <c r="K5" s="68">
+      <c r="K5" s="65">
         <v>0.16</v>
       </c>
-      <c r="L5" s="68">
+      <c r="L5" s="65">
         <v>0.17</v>
       </c>
-      <c r="M5" s="68">
+      <c r="M5" s="65">
         <v>0.18</v>
       </c>
-      <c r="N5" s="68">
+      <c r="N5" s="65">
         <v>0.19</v>
       </c>
-      <c r="O5" s="68">
+      <c r="O5" s="65">
         <v>0.2</v>
       </c>
-      <c r="P5" s="68">
+      <c r="P5" s="65">
         <v>0.21</v>
       </c>
-      <c r="Q5" s="68">
+      <c r="Q5" s="65">
         <v>0.22</v>
       </c>
-      <c r="R5" s="68">
+      <c r="R5" s="65">
         <v>0.23</v>
       </c>
-      <c r="S5" s="68">
+      <c r="S5" s="65">
         <v>0.24</v>
       </c>
       <c r="T5" s="11" t="s">
@@ -14646,23 +14786,23 @@
       <c r="U5" s="14"/>
     </row>
     <row r="6" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="66"/>
       <c r="T6" s="19"/>
       <c r="U6" s="40"/>
     </row>
@@ -14671,78 +14811,78 @@
         <v>82</v>
       </c>
       <c r="B7" s="46"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
       <c r="T7" s="21"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="65">
         <v>0.21</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="65">
         <v>0.22</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="65">
         <v>0.23</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="65">
         <v>0.24</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="65">
         <v>0.25</v>
       </c>
-      <c r="H8" s="68">
+      <c r="H8" s="65">
         <v>0.26</v>
       </c>
-      <c r="I8" s="68">
+      <c r="I8" s="65">
         <v>0.27</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K8" s="68">
+      <c r="K8" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L8" s="68">
+      <c r="L8" s="65">
         <v>0.3</v>
       </c>
-      <c r="M8" s="68">
+      <c r="M8" s="65">
         <v>0.31</v>
       </c>
-      <c r="N8" s="68">
+      <c r="N8" s="65">
         <v>0.32</v>
       </c>
-      <c r="O8" s="68">
+      <c r="O8" s="65">
         <v>0.33</v>
       </c>
-      <c r="P8" s="68">
+      <c r="P8" s="65">
         <v>0.34</v>
       </c>
-      <c r="Q8" s="68">
+      <c r="Q8" s="65">
         <v>0.35</v>
       </c>
-      <c r="R8" s="68">
+      <c r="R8" s="65">
         <v>0.36</v>
       </c>
-      <c r="S8" s="68">
+      <c r="S8" s="65">
         <v>0.37</v>
       </c>
       <c r="T8" s="11" t="s">
@@ -14754,55 +14894,55 @@
       <c r="B9" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="65">
         <v>0.18</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="65">
         <v>0.19</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="65">
         <v>0.2</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="65">
         <v>0.21</v>
       </c>
-      <c r="G9" s="68">
+      <c r="G9" s="65">
         <v>0.22</v>
       </c>
-      <c r="H9" s="68">
+      <c r="H9" s="65">
         <v>0.23</v>
       </c>
-      <c r="I9" s="68">
+      <c r="I9" s="65">
         <v>0.24</v>
       </c>
-      <c r="J9" s="68">
+      <c r="J9" s="65">
         <v>0.25</v>
       </c>
-      <c r="K9" s="68">
+      <c r="K9" s="65">
         <v>0.26</v>
       </c>
-      <c r="L9" s="68">
+      <c r="L9" s="65">
         <v>0.27</v>
       </c>
-      <c r="M9" s="68">
+      <c r="M9" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N9" s="68">
+      <c r="N9" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="O9" s="68">
+      <c r="O9" s="65">
         <v>0.3</v>
       </c>
-      <c r="P9" s="68">
+      <c r="P9" s="65">
         <v>0.31</v>
       </c>
-      <c r="Q9" s="68">
+      <c r="Q9" s="65">
         <v>0.32</v>
       </c>
-      <c r="R9" s="68">
+      <c r="R9" s="65">
         <v>0.33</v>
       </c>
-      <c r="S9" s="68">
+      <c r="S9" s="65">
         <v>0.34</v>
       </c>
       <c r="T9" s="11" t="s">
@@ -14814,55 +14954,55 @@
       <c r="B10" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="65">
         <v>0.16</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="65">
         <v>0.17</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="65">
         <v>0.18</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="65">
         <v>0.19</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="65">
         <v>0.2</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="65">
         <v>0.21</v>
       </c>
-      <c r="I10" s="68">
+      <c r="I10" s="65">
         <v>0.22</v>
       </c>
-      <c r="J10" s="68">
+      <c r="J10" s="65">
         <v>0.23</v>
       </c>
-      <c r="K10" s="68">
+      <c r="K10" s="65">
         <v>0.24</v>
       </c>
-      <c r="L10" s="68">
+      <c r="L10" s="65">
         <v>0.25</v>
       </c>
-      <c r="M10" s="68">
+      <c r="M10" s="65">
         <v>0.26</v>
       </c>
-      <c r="N10" s="68">
+      <c r="N10" s="65">
         <v>0.27</v>
       </c>
-      <c r="O10" s="68">
+      <c r="O10" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="P10" s="68">
+      <c r="P10" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q10" s="68">
+      <c r="Q10" s="65">
         <v>0.3</v>
       </c>
-      <c r="R10" s="68">
+      <c r="R10" s="65">
         <v>0.31</v>
       </c>
-      <c r="S10" s="68">
+      <c r="S10" s="65">
         <v>0.32</v>
       </c>
       <c r="T10" s="11" t="s">
@@ -14871,104 +15011,104 @@
       <c r="U10" s="27"/>
     </row>
     <row r="11" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="70"/>
-      <c r="N11" s="70"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="70"/>
-      <c r="Q11" s="70"/>
-      <c r="R11" s="70"/>
-      <c r="S11" s="70"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
       <c r="T11" s="19"/>
-      <c r="U11" s="63"/>
+      <c r="U11" s="60"/>
     </row>
     <row r="12" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="70"/>
-      <c r="P12" s="70"/>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="70"/>
-      <c r="S12" s="70"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
       <c r="T12" s="19"/>
-      <c r="U12" s="63"/>
+      <c r="U12" s="60"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="65">
         <v>0.3</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="65">
         <v>0.31</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="65">
         <v>0.32</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="65">
         <v>0.33</v>
       </c>
-      <c r="G13" s="68">
+      <c r="G13" s="65">
         <v>0.34</v>
       </c>
-      <c r="H13" s="68">
+      <c r="H13" s="65">
         <v>0.35</v>
       </c>
-      <c r="I13" s="68">
+      <c r="I13" s="65">
         <v>0.36</v>
       </c>
-      <c r="J13" s="68">
+      <c r="J13" s="65">
         <v>0.37</v>
       </c>
-      <c r="K13" s="68">
+      <c r="K13" s="65">
         <v>0.38</v>
       </c>
-      <c r="L13" s="68">
+      <c r="L13" s="65">
         <v>0.39</v>
       </c>
-      <c r="M13" s="68">
+      <c r="M13" s="65">
         <v>0.4</v>
       </c>
-      <c r="N13" s="68">
+      <c r="N13" s="65">
         <v>0.41</v>
       </c>
-      <c r="O13" s="68">
+      <c r="O13" s="65">
         <v>0.42</v>
       </c>
-      <c r="P13" s="68">
+      <c r="P13" s="65">
         <v>0.43</v>
       </c>
-      <c r="Q13" s="68">
+      <c r="Q13" s="65">
         <v>0.44</v>
       </c>
-      <c r="R13" s="68">
+      <c r="R13" s="65">
         <v>0.45</v>
       </c>
-      <c r="S13" s="68">
+      <c r="S13" s="65">
         <v>0.46</v>
       </c>
       <c r="T13" s="11" t="s">
@@ -14980,55 +15120,55 @@
       <c r="B14" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="68">
+      <c r="C14" s="65">
         <v>0.45</v>
       </c>
-      <c r="D14" s="68">
+      <c r="D14" s="65">
         <v>0.46</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="65">
         <v>0.47</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="65">
         <v>0.48</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="65">
         <v>0.49</v>
       </c>
-      <c r="H14" s="68">
+      <c r="H14" s="65">
         <v>0.5</v>
       </c>
-      <c r="I14" s="68">
+      <c r="I14" s="65">
         <v>0.51</v>
       </c>
-      <c r="J14" s="68">
+      <c r="J14" s="65">
         <v>0.52</v>
       </c>
-      <c r="K14" s="68">
+      <c r="K14" s="65">
         <v>0.53</v>
       </c>
-      <c r="L14" s="68">
+      <c r="L14" s="65">
         <v>0.54</v>
       </c>
-      <c r="M14" s="68">
+      <c r="M14" s="65">
         <v>0.55000000000000004</v>
       </c>
-      <c r="N14" s="68">
+      <c r="N14" s="65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="O14" s="68">
+      <c r="O14" s="65">
         <v>0.56999999999999995</v>
       </c>
-      <c r="P14" s="68">
+      <c r="P14" s="65">
         <v>0.57999999999999996</v>
       </c>
-      <c r="Q14" s="68">
+      <c r="Q14" s="65">
         <v>0.59</v>
       </c>
-      <c r="R14" s="68">
+      <c r="R14" s="65">
         <v>0.6</v>
       </c>
-      <c r="S14" s="68">
+      <c r="S14" s="65">
         <v>0.61</v>
       </c>
       <c r="T14" s="11" t="s">
@@ -15040,161 +15180,161 @@
       <c r="B15" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="68">
+      <c r="C15" s="65">
         <v>0.24</v>
       </c>
-      <c r="D15" s="68">
+      <c r="D15" s="65">
         <v>0.23</v>
       </c>
-      <c r="E15" s="68">
+      <c r="E15" s="65">
         <v>0.22</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="65">
         <v>0.21</v>
       </c>
-      <c r="G15" s="68">
+      <c r="G15" s="65">
         <v>0.2</v>
       </c>
-      <c r="H15" s="68">
+      <c r="H15" s="65">
         <v>0.19</v>
       </c>
-      <c r="I15" s="68">
+      <c r="I15" s="65">
         <v>0.18</v>
       </c>
-      <c r="J15" s="68">
+      <c r="J15" s="65">
         <v>0.17</v>
       </c>
-      <c r="K15" s="68">
+      <c r="K15" s="65">
         <v>0.16</v>
       </c>
-      <c r="L15" s="68">
+      <c r="L15" s="65">
         <v>0.15</v>
       </c>
-      <c r="M15" s="68">
+      <c r="M15" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N15" s="68">
+      <c r="N15" s="65">
         <v>0.13</v>
       </c>
-      <c r="O15" s="68">
+      <c r="O15" s="65">
         <v>0.12</v>
       </c>
-      <c r="P15" s="68">
+      <c r="P15" s="65">
         <v>0.11</v>
       </c>
-      <c r="Q15" s="68">
+      <c r="Q15" s="65">
         <v>0.1</v>
       </c>
-      <c r="R15" s="68">
+      <c r="R15" s="65">
         <v>0.09</v>
       </c>
-      <c r="S15" s="68">
+      <c r="S15" s="65">
         <v>0.08</v>
       </c>
       <c r="T15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U15" s="65"/>
+      <c r="U15" s="62"/>
     </row>
     <row r="16" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="70"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="70"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="70"/>
-      <c r="S16" s="70"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="67"/>
+      <c r="S16" s="67"/>
       <c r="T16" s="19"/>
-      <c r="U16" s="63"/>
+      <c r="U16" s="60"/>
     </row>
     <row r="17" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="70"/>
-      <c r="S17" s="70"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="67"/>
+      <c r="S17" s="67"/>
       <c r="T17" s="19"/>
-      <c r="U17" s="63"/>
+      <c r="U17" s="60"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="68">
+      <c r="C18" s="65">
         <v>0.67</v>
       </c>
-      <c r="D18" s="68">
+      <c r="D18" s="65">
         <v>0.68</v>
       </c>
-      <c r="E18" s="68">
+      <c r="E18" s="65">
         <v>0.69</v>
       </c>
-      <c r="F18" s="68">
+      <c r="F18" s="65">
         <v>0.7</v>
       </c>
-      <c r="G18" s="68">
+      <c r="G18" s="65">
         <v>0.71</v>
       </c>
-      <c r="H18" s="68">
+      <c r="H18" s="65">
         <v>0.72</v>
       </c>
-      <c r="I18" s="68">
+      <c r="I18" s="65">
         <v>0.73</v>
       </c>
-      <c r="J18" s="68">
+      <c r="J18" s="65">
         <v>0.74</v>
       </c>
-      <c r="K18" s="68">
+      <c r="K18" s="65">
         <v>0.75</v>
       </c>
-      <c r="L18" s="68">
+      <c r="L18" s="65">
         <v>0.76</v>
       </c>
-      <c r="M18" s="68">
+      <c r="M18" s="65">
         <v>0.77</v>
       </c>
-      <c r="N18" s="68">
+      <c r="N18" s="65">
         <v>0.78</v>
       </c>
-      <c r="O18" s="68">
+      <c r="O18" s="65">
         <v>0.79</v>
       </c>
-      <c r="P18" s="68">
+      <c r="P18" s="65">
         <v>0.8</v>
       </c>
-      <c r="Q18" s="68">
+      <c r="Q18" s="65">
         <v>0.81</v>
       </c>
-      <c r="R18" s="68">
+      <c r="R18" s="65">
         <v>0.82</v>
       </c>
-      <c r="S18" s="68">
+      <c r="S18" s="65">
         <v>0.83</v>
       </c>
       <c r="T18" s="11" t="s">
@@ -15203,58 +15343,58 @@
       <c r="U18" s="14"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="68">
+      <c r="C19" s="65">
         <v>0.65</v>
       </c>
-      <c r="D19" s="68">
+      <c r="D19" s="65">
         <v>0.66</v>
       </c>
-      <c r="E19" s="68">
+      <c r="E19" s="65">
         <v>0.67</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="65">
         <v>0.68</v>
       </c>
-      <c r="G19" s="68">
+      <c r="G19" s="65">
         <v>0.69</v>
       </c>
-      <c r="H19" s="68">
+      <c r="H19" s="65">
         <v>0.7</v>
       </c>
-      <c r="I19" s="68">
+      <c r="I19" s="65">
         <v>0.71</v>
       </c>
-      <c r="J19" s="68">
+      <c r="J19" s="65">
         <v>0.72</v>
       </c>
-      <c r="K19" s="68">
+      <c r="K19" s="65">
         <v>0.73</v>
       </c>
-      <c r="L19" s="68">
+      <c r="L19" s="65">
         <v>0.74</v>
       </c>
-      <c r="M19" s="68">
+      <c r="M19" s="65">
         <v>0.75</v>
       </c>
-      <c r="N19" s="68">
+      <c r="N19" s="65">
         <v>0.76</v>
       </c>
-      <c r="O19" s="68">
+      <c r="O19" s="65">
         <v>0.77</v>
       </c>
-      <c r="P19" s="68">
+      <c r="P19" s="65">
         <v>0.78</v>
       </c>
-      <c r="Q19" s="68">
+      <c r="Q19" s="65">
         <v>0.79</v>
       </c>
-      <c r="R19" s="68">
+      <c r="R19" s="65">
         <v>0.8</v>
       </c>
-      <c r="S19" s="68">
+      <c r="S19" s="65">
         <v>0.81</v>
       </c>
       <c r="T19" s="11" t="s">
@@ -15263,58 +15403,58 @@
       <c r="U19" s="14"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="68">
+      <c r="C20" s="65">
         <v>0.64</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="65">
         <v>0.65</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="65">
         <v>0.66</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="65">
         <v>0.67</v>
       </c>
-      <c r="G20" s="68">
+      <c r="G20" s="65">
         <v>0.68</v>
       </c>
-      <c r="H20" s="68">
+      <c r="H20" s="65">
         <v>0.69</v>
       </c>
-      <c r="I20" s="68">
+      <c r="I20" s="65">
         <v>0.7</v>
       </c>
-      <c r="J20" s="68">
+      <c r="J20" s="65">
         <v>0.71</v>
       </c>
-      <c r="K20" s="68">
+      <c r="K20" s="65">
         <v>0.72</v>
       </c>
-      <c r="L20" s="68">
+      <c r="L20" s="65">
         <v>0.73</v>
       </c>
-      <c r="M20" s="68">
+      <c r="M20" s="65">
         <v>0.74</v>
       </c>
-      <c r="N20" s="68">
+      <c r="N20" s="65">
         <v>0.75</v>
       </c>
-      <c r="O20" s="68">
+      <c r="O20" s="65">
         <v>0.76</v>
       </c>
-      <c r="P20" s="68">
+      <c r="P20" s="65">
         <v>0.77</v>
       </c>
-      <c r="Q20" s="68">
+      <c r="Q20" s="65">
         <v>0.78</v>
       </c>
-      <c r="R20" s="68">
+      <c r="R20" s="65">
         <v>0.79</v>
       </c>
-      <c r="S20" s="68">
+      <c r="S20" s="65">
         <v>0.8</v>
       </c>
       <c r="T20" s="11" t="s">
@@ -15323,79 +15463,79 @@
       <c r="U20" s="14"/>
     </row>
     <row r="21" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="70"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="70"/>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="70"/>
-      <c r="S21" s="70"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
       <c r="T21" s="19"/>
-      <c r="U21" s="63"/>
+      <c r="U21" s="60"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="68">
+      <c r="C22" s="65">
         <v>0.35</v>
       </c>
-      <c r="D22" s="68">
+      <c r="D22" s="65">
         <v>0.36</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="65">
         <v>0.37</v>
       </c>
-      <c r="F22" s="68">
+      <c r="F22" s="65">
         <v>0.38</v>
       </c>
-      <c r="G22" s="68">
+      <c r="G22" s="65">
         <v>0.39</v>
       </c>
-      <c r="H22" s="68">
+      <c r="H22" s="65">
         <v>0.4</v>
       </c>
-      <c r="I22" s="68">
+      <c r="I22" s="65">
         <v>0.41</v>
       </c>
-      <c r="J22" s="68">
+      <c r="J22" s="65">
         <v>0.42</v>
       </c>
-      <c r="K22" s="68">
+      <c r="K22" s="65">
         <v>0.43</v>
       </c>
-      <c r="L22" s="68">
+      <c r="L22" s="65">
         <v>0.44</v>
       </c>
-      <c r="M22" s="68">
+      <c r="M22" s="65">
         <v>0.45</v>
       </c>
-      <c r="N22" s="68">
+      <c r="N22" s="65">
         <v>0.46</v>
       </c>
-      <c r="O22" s="68">
+      <c r="O22" s="65">
         <v>0.47</v>
       </c>
-      <c r="P22" s="68">
+      <c r="P22" s="65">
         <v>0.48</v>
       </c>
-      <c r="Q22" s="68">
+      <c r="Q22" s="65">
         <v>0.49</v>
       </c>
-      <c r="R22" s="68">
+      <c r="R22" s="65">
         <v>0.5</v>
       </c>
-      <c r="S22" s="68">
+      <c r="S22" s="65">
         <v>0.51</v>
       </c>
       <c r="T22" s="11" t="s">
@@ -15404,58 +15544,58 @@
       <c r="U22" s="14"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="68">
+      <c r="C23" s="65">
         <v>0.33</v>
       </c>
-      <c r="D23" s="68">
+      <c r="D23" s="65">
         <v>0.32</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="65">
         <v>0.31</v>
       </c>
-      <c r="F23" s="68">
+      <c r="F23" s="65">
         <v>0.3</v>
       </c>
-      <c r="G23" s="68">
+      <c r="G23" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H23" s="68">
+      <c r="H23" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I23" s="68">
+      <c r="I23" s="65">
         <v>0.27</v>
       </c>
-      <c r="J23" s="68">
+      <c r="J23" s="65">
         <v>0.26</v>
       </c>
-      <c r="K23" s="68">
+      <c r="K23" s="65">
         <v>0.25</v>
       </c>
-      <c r="L23" s="68">
+      <c r="L23" s="65">
         <v>0.24</v>
       </c>
-      <c r="M23" s="68">
+      <c r="M23" s="65">
         <v>0.23</v>
       </c>
-      <c r="N23" s="68">
+      <c r="N23" s="65">
         <v>0.22</v>
       </c>
-      <c r="O23" s="68">
+      <c r="O23" s="65">
         <v>0.21</v>
       </c>
-      <c r="P23" s="68">
+      <c r="P23" s="65">
         <v>0.2</v>
       </c>
-      <c r="Q23" s="68">
+      <c r="Q23" s="65">
         <v>0.19</v>
       </c>
-      <c r="R23" s="68">
+      <c r="R23" s="65">
         <v>0.18</v>
       </c>
-      <c r="S23" s="68">
+      <c r="S23" s="65">
         <v>0.17</v>
       </c>
       <c r="T23" s="11" t="s">
@@ -15464,58 +15604,58 @@
       <c r="U23" s="14"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="68">
+      <c r="C24" s="65">
         <v>0.31</v>
       </c>
-      <c r="D24" s="68">
+      <c r="D24" s="65">
         <v>0.3</v>
       </c>
-      <c r="E24" s="68">
+      <c r="E24" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G24" s="68">
+      <c r="G24" s="65">
         <v>0.27</v>
       </c>
-      <c r="H24" s="68">
+      <c r="H24" s="65">
         <v>0.26</v>
       </c>
-      <c r="I24" s="68">
+      <c r="I24" s="65">
         <v>0.25</v>
       </c>
-      <c r="J24" s="68">
+      <c r="J24" s="65">
         <v>0.24</v>
       </c>
-      <c r="K24" s="68">
+      <c r="K24" s="65">
         <v>0.23</v>
       </c>
-      <c r="L24" s="68">
+      <c r="L24" s="65">
         <v>0.22</v>
       </c>
-      <c r="M24" s="68">
+      <c r="M24" s="65">
         <v>0.21</v>
       </c>
-      <c r="N24" s="68">
+      <c r="N24" s="65">
         <v>0.2</v>
       </c>
-      <c r="O24" s="68">
+      <c r="O24" s="65">
         <v>0.19</v>
       </c>
-      <c r="P24" s="68">
+      <c r="P24" s="65">
         <v>0.18</v>
       </c>
-      <c r="Q24" s="68">
+      <c r="Q24" s="65">
         <v>0.17</v>
       </c>
-      <c r="R24" s="68">
+      <c r="R24" s="65">
         <v>0.16</v>
       </c>
-      <c r="S24" s="68">
+      <c r="S24" s="65">
         <v>0.15</v>
       </c>
       <c r="T24" s="11" t="s">
@@ -15524,79 +15664,79 @@
       <c r="U24" s="14"/>
     </row>
     <row r="25" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="70"/>
-      <c r="M25" s="70"/>
-      <c r="N25" s="70"/>
-      <c r="O25" s="70"/>
-      <c r="P25" s="70"/>
-      <c r="Q25" s="70"/>
-      <c r="R25" s="70"/>
-      <c r="S25" s="70"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="67"/>
+      <c r="S25" s="67"/>
       <c r="T25" s="19"/>
-      <c r="U25" s="63"/>
+      <c r="U25" s="60"/>
     </row>
     <row r="26" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="68">
+      <c r="C26" s="65">
         <v>0.66</v>
       </c>
-      <c r="D26" s="68">
+      <c r="D26" s="65">
         <v>0.65</v>
       </c>
-      <c r="E26" s="68">
+      <c r="E26" s="65">
         <v>0.64</v>
       </c>
-      <c r="F26" s="68">
+      <c r="F26" s="65">
         <v>0.63</v>
       </c>
-      <c r="G26" s="68">
+      <c r="G26" s="65">
         <v>0.62</v>
       </c>
-      <c r="H26" s="68">
+      <c r="H26" s="65">
         <v>0.61</v>
       </c>
-      <c r="I26" s="68">
+      <c r="I26" s="65">
         <v>0.6</v>
       </c>
-      <c r="J26" s="68">
+      <c r="J26" s="65">
         <v>0.59</v>
       </c>
-      <c r="K26" s="68">
+      <c r="K26" s="65">
         <v>0.57999999999999996</v>
       </c>
-      <c r="L26" s="68">
+      <c r="L26" s="65">
         <v>0.56999999999999995</v>
       </c>
-      <c r="M26" s="68">
+      <c r="M26" s="65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="N26" s="68">
+      <c r="N26" s="65">
         <v>0.55000000000000004</v>
       </c>
-      <c r="O26" s="68">
+      <c r="O26" s="65">
         <v>0.54</v>
       </c>
-      <c r="P26" s="68">
+      <c r="P26" s="65">
         <v>0.53</v>
       </c>
-      <c r="Q26" s="68">
+      <c r="Q26" s="65">
         <v>0.52</v>
       </c>
-      <c r="R26" s="68">
+      <c r="R26" s="65">
         <v>0.51</v>
       </c>
-      <c r="S26" s="68">
+      <c r="S26" s="65">
         <v>0.5</v>
       </c>
       <c r="T26" s="11" t="s">
@@ -15605,58 +15745,58 @@
       <c r="U26" s="14"/>
     </row>
     <row r="27" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="68">
+      <c r="C27" s="65">
         <v>0.63</v>
       </c>
-      <c r="D27" s="68">
+      <c r="D27" s="65">
         <v>0.62</v>
       </c>
-      <c r="E27" s="68">
+      <c r="E27" s="65">
         <v>0.61</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="65">
         <v>0.6</v>
       </c>
-      <c r="G27" s="68">
+      <c r="G27" s="65">
         <v>0.59</v>
       </c>
-      <c r="H27" s="68">
+      <c r="H27" s="65">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I27" s="68">
+      <c r="I27" s="65">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J27" s="68">
+      <c r="J27" s="65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="K27" s="68">
+      <c r="K27" s="65">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L27" s="68">
+      <c r="L27" s="65">
         <v>0.54</v>
       </c>
-      <c r="M27" s="68">
+      <c r="M27" s="65">
         <v>0.53</v>
       </c>
-      <c r="N27" s="68">
+      <c r="N27" s="65">
         <v>0.52</v>
       </c>
-      <c r="O27" s="68">
+      <c r="O27" s="65">
         <v>0.51</v>
       </c>
-      <c r="P27" s="68">
+      <c r="P27" s="65">
         <v>0.5</v>
       </c>
-      <c r="Q27" s="68">
+      <c r="Q27" s="65">
         <v>0.49</v>
       </c>
-      <c r="R27" s="68">
+      <c r="R27" s="65">
         <v>0.48</v>
       </c>
-      <c r="S27" s="68">
+      <c r="S27" s="65">
         <v>0.47</v>
       </c>
       <c r="T27" s="11" t="s">
@@ -15665,163 +15805,163 @@
       <c r="U27" s="14"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="68">
+      <c r="C28" s="65">
         <v>0.61</v>
       </c>
-      <c r="D28" s="68">
+      <c r="D28" s="65">
         <v>0.6</v>
       </c>
-      <c r="E28" s="68">
+      <c r="E28" s="65">
         <v>0.59</v>
       </c>
-      <c r="F28" s="68">
+      <c r="F28" s="65">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G28" s="68">
+      <c r="G28" s="65">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H28" s="68">
+      <c r="H28" s="65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I28" s="68">
+      <c r="I28" s="65">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J28" s="68">
+      <c r="J28" s="65">
         <v>0.54</v>
       </c>
-      <c r="K28" s="68">
+      <c r="K28" s="65">
         <v>0.53</v>
       </c>
-      <c r="L28" s="68">
+      <c r="L28" s="65">
         <v>0.52</v>
       </c>
-      <c r="M28" s="68">
+      <c r="M28" s="65">
         <v>0.51</v>
       </c>
-      <c r="N28" s="68">
+      <c r="N28" s="65">
         <v>0.5</v>
       </c>
-      <c r="O28" s="68">
+      <c r="O28" s="65">
         <v>0.49</v>
       </c>
-      <c r="P28" s="68">
+      <c r="P28" s="65">
         <v>0.48</v>
       </c>
-      <c r="Q28" s="68">
+      <c r="Q28" s="65">
         <v>0.47</v>
       </c>
-      <c r="R28" s="68">
+      <c r="R28" s="65">
         <v>0.46</v>
       </c>
-      <c r="S28" s="68">
+      <c r="S28" s="65">
         <v>0.45</v>
       </c>
       <c r="T28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U28" s="65"/>
-    </row>
-    <row r="29" spans="1:21" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="71"/>
-      <c r="K29" s="71"/>
-      <c r="L29" s="71"/>
-      <c r="M29" s="71"/>
-      <c r="N29" s="71"/>
-      <c r="O29" s="71"/>
-      <c r="P29" s="71"/>
-      <c r="Q29" s="71"/>
-      <c r="R29" s="71"/>
-      <c r="S29" s="71"/>
+      <c r="U28" s="62"/>
+    </row>
+    <row r="29" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="68"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="68"/>
+      <c r="Q29" s="68"/>
+      <c r="R29" s="68"/>
+      <c r="S29" s="68"/>
       <c r="T29" s="38"/>
-      <c r="U29" s="67"/>
+      <c r="U29" s="64"/>
     </row>
     <row r="30" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="70"/>
-      <c r="M30" s="70"/>
-      <c r="N30" s="70"/>
-      <c r="O30" s="70"/>
-      <c r="P30" s="70"/>
-      <c r="Q30" s="70"/>
-      <c r="R30" s="70"/>
-      <c r="S30" s="70"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="67"/>
+      <c r="P30" s="67"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="67"/>
+      <c r="S30" s="67"/>
       <c r="T30" s="19"/>
-      <c r="U30" s="63"/>
+      <c r="U30" s="60"/>
     </row>
     <row r="31" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="68">
+      <c r="C31" s="65">
         <v>0.68</v>
       </c>
-      <c r="D31" s="68">
+      <c r="D31" s="65">
         <v>0.69</v>
       </c>
-      <c r="E31" s="68">
+      <c r="E31" s="65">
         <v>0.7</v>
       </c>
-      <c r="F31" s="68">
+      <c r="F31" s="65">
         <v>0.71</v>
       </c>
-      <c r="G31" s="68">
+      <c r="G31" s="65">
         <v>0.72</v>
       </c>
-      <c r="H31" s="68">
+      <c r="H31" s="65">
         <v>0.73</v>
       </c>
-      <c r="I31" s="68">
+      <c r="I31" s="65">
         <v>0.73999999999999899</v>
       </c>
-      <c r="J31" s="68">
+      <c r="J31" s="65">
         <v>0.749999999999999</v>
       </c>
-      <c r="K31" s="68">
+      <c r="K31" s="65">
         <v>0.75999999999999901</v>
       </c>
-      <c r="L31" s="68">
+      <c r="L31" s="65">
         <v>0.76999999999999902</v>
       </c>
-      <c r="M31" s="68">
+      <c r="M31" s="65">
         <v>0.77999999999999903</v>
       </c>
-      <c r="N31" s="68">
+      <c r="N31" s="65">
         <v>0.78999999999999904</v>
       </c>
-      <c r="O31" s="68">
+      <c r="O31" s="65">
         <v>0.79999999999999905</v>
       </c>
-      <c r="P31" s="68">
+      <c r="P31" s="65">
         <v>0.80999999999999905</v>
       </c>
-      <c r="Q31" s="68">
+      <c r="Q31" s="65">
         <v>0.81999999999999895</v>
       </c>
-      <c r="R31" s="68">
+      <c r="R31" s="65">
         <v>0.82999999999999796</v>
       </c>
-      <c r="S31" s="68">
+      <c r="S31" s="65">
         <v>0.83999999999999797</v>
       </c>
       <c r="T31" s="11" t="s">
@@ -15830,58 +15970,58 @@
       <c r="U31" s="14"/>
     </row>
     <row r="32" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="68">
+      <c r="C32" s="65">
         <v>0.66</v>
       </c>
-      <c r="D32" s="68">
+      <c r="D32" s="65">
         <v>0.65</v>
       </c>
-      <c r="E32" s="68">
+      <c r="E32" s="65">
         <v>0.64</v>
       </c>
-      <c r="F32" s="68">
+      <c r="F32" s="65">
         <v>0.63</v>
       </c>
-      <c r="G32" s="68">
+      <c r="G32" s="65">
         <v>0.62</v>
       </c>
-      <c r="H32" s="68">
+      <c r="H32" s="65">
         <v>0.61</v>
       </c>
-      <c r="I32" s="68">
+      <c r="I32" s="65">
         <v>0.6</v>
       </c>
-      <c r="J32" s="68">
+      <c r="J32" s="65">
         <v>0.59</v>
       </c>
-      <c r="K32" s="68">
+      <c r="K32" s="65">
         <v>0.57999999999999996</v>
       </c>
-      <c r="L32" s="68">
+      <c r="L32" s="65">
         <v>0.56999999999999995</v>
       </c>
-      <c r="M32" s="68">
+      <c r="M32" s="65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="N32" s="68">
+      <c r="N32" s="65">
         <v>0.55000000000000004</v>
       </c>
-      <c r="O32" s="68">
+      <c r="O32" s="65">
         <v>0.54</v>
       </c>
-      <c r="P32" s="68">
+      <c r="P32" s="65">
         <v>0.53</v>
       </c>
-      <c r="Q32" s="68">
+      <c r="Q32" s="65">
         <v>0.52</v>
       </c>
-      <c r="R32" s="68">
+      <c r="R32" s="65">
         <v>0.51</v>
       </c>
-      <c r="S32" s="68">
+      <c r="S32" s="65">
         <v>0.5</v>
       </c>
       <c r="T32" s="11" t="s">
@@ -15890,58 +16030,58 @@
       <c r="U32" s="14"/>
     </row>
     <row r="33" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="68">
+      <c r="C33" s="65">
         <v>0.64</v>
       </c>
-      <c r="D33" s="68">
+      <c r="D33" s="65">
         <v>0.63</v>
       </c>
-      <c r="E33" s="68">
+      <c r="E33" s="65">
         <v>0.62</v>
       </c>
-      <c r="F33" s="68">
+      <c r="F33" s="65">
         <v>0.61</v>
       </c>
-      <c r="G33" s="68">
+      <c r="G33" s="65">
         <v>0.6</v>
       </c>
-      <c r="H33" s="68">
+      <c r="H33" s="65">
         <v>0.59</v>
       </c>
-      <c r="I33" s="68">
+      <c r="I33" s="65">
         <v>0.57999999999999996</v>
       </c>
-      <c r="J33" s="68">
+      <c r="J33" s="65">
         <v>0.56999999999999995</v>
       </c>
-      <c r="K33" s="68">
+      <c r="K33" s="65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L33" s="68">
+      <c r="L33" s="65">
         <v>0.55000000000000004</v>
       </c>
-      <c r="M33" s="68">
+      <c r="M33" s="65">
         <v>0.54</v>
       </c>
-      <c r="N33" s="68">
+      <c r="N33" s="65">
         <v>0.53</v>
       </c>
-      <c r="O33" s="68">
+      <c r="O33" s="65">
         <v>0.52</v>
       </c>
-      <c r="P33" s="68">
+      <c r="P33" s="65">
         <v>0.51</v>
       </c>
-      <c r="Q33" s="68">
+      <c r="Q33" s="65">
         <v>0.5</v>
       </c>
-      <c r="R33" s="68">
+      <c r="R33" s="65">
         <v>0.49</v>
       </c>
-      <c r="S33" s="68">
+      <c r="S33" s="65">
         <v>0.48</v>
       </c>
       <c r="T33" s="11" t="s">
@@ -15950,79 +16090,79 @@
       <c r="U33" s="14"/>
     </row>
     <row r="34" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="67"/>
+      <c r="S34" s="67"/>
       <c r="T34" s="19"/>
-      <c r="U34" s="63"/>
+      <c r="U34" s="60"/>
     </row>
     <row r="35" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="68">
+      <c r="C35" s="65">
         <v>0.85</v>
       </c>
-      <c r="D35" s="68">
+      <c r="D35" s="65">
         <v>0.86</v>
       </c>
-      <c r="E35" s="68">
+      <c r="E35" s="65">
         <v>0.87</v>
       </c>
-      <c r="F35" s="68">
+      <c r="F35" s="65">
         <v>0.88</v>
       </c>
-      <c r="G35" s="68">
+      <c r="G35" s="65">
         <v>0.89</v>
       </c>
-      <c r="H35" s="68">
+      <c r="H35" s="65">
         <v>0.9</v>
       </c>
-      <c r="I35" s="68">
+      <c r="I35" s="65">
         <v>0.91</v>
       </c>
-      <c r="J35" s="68">
+      <c r="J35" s="65">
         <v>0.92</v>
       </c>
-      <c r="K35" s="68">
+      <c r="K35" s="65">
         <v>0.93</v>
       </c>
-      <c r="L35" s="68">
+      <c r="L35" s="65">
         <v>0.94</v>
       </c>
-      <c r="M35" s="68">
+      <c r="M35" s="65">
         <v>0.95</v>
       </c>
-      <c r="N35" s="68">
+      <c r="N35" s="65">
         <v>0.96</v>
       </c>
-      <c r="O35" s="68">
+      <c r="O35" s="65">
         <v>0.97</v>
       </c>
-      <c r="P35" s="68">
+      <c r="P35" s="65">
         <v>0.98</v>
       </c>
-      <c r="Q35" s="68">
+      <c r="Q35" s="65">
         <v>0.99</v>
       </c>
-      <c r="R35" s="68">
+      <c r="R35" s="65">
         <v>1</v>
       </c>
-      <c r="S35" s="68">
+      <c r="S35" s="65">
         <v>1.01</v>
       </c>
       <c r="T35" s="11" t="s">
@@ -16031,58 +16171,58 @@
       <c r="U35" s="14"/>
     </row>
     <row r="36" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="68">
+      <c r="C36" s="65">
         <v>0.84</v>
       </c>
-      <c r="D36" s="68">
+      <c r="D36" s="65">
         <v>0.83</v>
       </c>
-      <c r="E36" s="68">
+      <c r="E36" s="65">
         <v>0.82</v>
       </c>
-      <c r="F36" s="68">
+      <c r="F36" s="65">
         <v>0.81</v>
       </c>
-      <c r="G36" s="68">
+      <c r="G36" s="65">
         <v>0.8</v>
       </c>
-      <c r="H36" s="68">
+      <c r="H36" s="65">
         <v>0.79</v>
       </c>
-      <c r="I36" s="68">
+      <c r="I36" s="65">
         <v>0.78</v>
       </c>
-      <c r="J36" s="68">
+      <c r="J36" s="65">
         <v>0.77</v>
       </c>
-      <c r="K36" s="68">
+      <c r="K36" s="65">
         <v>0.76</v>
       </c>
-      <c r="L36" s="68">
+      <c r="L36" s="65">
         <v>0.75</v>
       </c>
-      <c r="M36" s="68">
+      <c r="M36" s="65">
         <v>0.74</v>
       </c>
-      <c r="N36" s="68">
+      <c r="N36" s="65">
         <v>0.73</v>
       </c>
-      <c r="O36" s="68">
+      <c r="O36" s="65">
         <v>0.72</v>
       </c>
-      <c r="P36" s="68">
+      <c r="P36" s="65">
         <v>0.71</v>
       </c>
-      <c r="Q36" s="68">
+      <c r="Q36" s="65">
         <v>0.7</v>
       </c>
-      <c r="R36" s="68">
+      <c r="R36" s="65">
         <v>0.69</v>
       </c>
-      <c r="S36" s="68">
+      <c r="S36" s="65">
         <v>0.68</v>
       </c>
       <c r="T36" s="11" t="s">
@@ -16091,58 +16231,58 @@
       <c r="U36" s="14"/>
     </row>
     <row r="37" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="68">
+      <c r="C37" s="65">
         <v>0.82</v>
       </c>
-      <c r="D37" s="68">
+      <c r="D37" s="65">
         <v>0.81</v>
       </c>
-      <c r="E37" s="68">
+      <c r="E37" s="65">
         <v>0.8</v>
       </c>
-      <c r="F37" s="68">
+      <c r="F37" s="65">
         <v>0.79</v>
       </c>
-      <c r="G37" s="68">
+      <c r="G37" s="65">
         <v>0.78</v>
       </c>
-      <c r="H37" s="68">
+      <c r="H37" s="65">
         <v>0.77</v>
       </c>
-      <c r="I37" s="68">
+      <c r="I37" s="65">
         <v>0.76000000000000101</v>
       </c>
-      <c r="J37" s="68">
+      <c r="J37" s="65">
         <v>0.750000000000001</v>
       </c>
-      <c r="K37" s="68">
+      <c r="K37" s="65">
         <v>0.74000000000000099</v>
       </c>
-      <c r="L37" s="68">
+      <c r="L37" s="65">
         <v>0.73000000000000098</v>
       </c>
-      <c r="M37" s="68">
+      <c r="M37" s="65">
         <v>0.72000000000000097</v>
       </c>
-      <c r="N37" s="68">
+      <c r="N37" s="65">
         <v>0.71000000000000096</v>
       </c>
-      <c r="O37" s="68">
+      <c r="O37" s="65">
         <v>0.70000000000000095</v>
       </c>
-      <c r="P37" s="68">
+      <c r="P37" s="65">
         <v>0.69000000000000095</v>
       </c>
-      <c r="Q37" s="68">
+      <c r="Q37" s="65">
         <v>0.68000000000000105</v>
       </c>
-      <c r="R37" s="68">
+      <c r="R37" s="65">
         <v>0.67000000000000204</v>
       </c>
-      <c r="S37" s="68">
+      <c r="S37" s="65">
         <v>0.66000000000000203</v>
       </c>
       <c r="T37" s="11" t="s">
@@ -16151,79 +16291,79 @@
       <c r="U37" s="14"/>
     </row>
     <row r="38" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
-      <c r="O38" s="70"/>
-      <c r="P38" s="70"/>
-      <c r="Q38" s="70"/>
-      <c r="R38" s="70"/>
-      <c r="S38" s="70"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="67"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="67"/>
+      <c r="O38" s="67"/>
+      <c r="P38" s="67"/>
+      <c r="Q38" s="67"/>
+      <c r="R38" s="67"/>
+      <c r="S38" s="67"/>
       <c r="T38" s="19"/>
-      <c r="U38" s="63"/>
+      <c r="U38" s="60"/>
     </row>
     <row r="39" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="62" t="s">
+      <c r="B39" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="68">
+      <c r="C39" s="65">
         <v>0.74</v>
       </c>
-      <c r="D39" s="68">
+      <c r="D39" s="65">
         <v>0.73</v>
       </c>
-      <c r="E39" s="68">
+      <c r="E39" s="65">
         <v>0.72</v>
       </c>
-      <c r="F39" s="68">
+      <c r="F39" s="65">
         <v>0.71</v>
       </c>
-      <c r="G39" s="68">
+      <c r="G39" s="65">
         <v>0.7</v>
       </c>
-      <c r="H39" s="68">
+      <c r="H39" s="65">
         <v>0.69</v>
       </c>
-      <c r="I39" s="68">
+      <c r="I39" s="65">
         <v>0.68</v>
       </c>
-      <c r="J39" s="68">
+      <c r="J39" s="65">
         <v>0.67</v>
       </c>
-      <c r="K39" s="68">
+      <c r="K39" s="65">
         <v>0.66</v>
       </c>
-      <c r="L39" s="68">
+      <c r="L39" s="65">
         <v>0.65</v>
       </c>
-      <c r="M39" s="68">
+      <c r="M39" s="65">
         <v>0.64</v>
       </c>
-      <c r="N39" s="68">
+      <c r="N39" s="65">
         <v>0.63</v>
       </c>
-      <c r="O39" s="68">
+      <c r="O39" s="65">
         <v>0.62</v>
       </c>
-      <c r="P39" s="68">
+      <c r="P39" s="65">
         <v>0.61</v>
       </c>
-      <c r="Q39" s="68">
+      <c r="Q39" s="65">
         <v>0.6</v>
       </c>
-      <c r="R39" s="68">
+      <c r="R39" s="65">
         <v>0.59</v>
       </c>
-      <c r="S39" s="68">
+      <c r="S39" s="65">
         <v>0.57999999999999996</v>
       </c>
       <c r="T39" s="11" t="s">
@@ -16232,58 +16372,58 @@
       <c r="U39" s="14"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B40" s="62" t="s">
+      <c r="B40" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="68">
+      <c r="C40" s="65">
         <v>0.72</v>
       </c>
-      <c r="D40" s="68">
+      <c r="D40" s="65">
         <v>0.71</v>
       </c>
-      <c r="E40" s="68">
+      <c r="E40" s="65">
         <v>0.7</v>
       </c>
-      <c r="F40" s="68">
+      <c r="F40" s="65">
         <v>0.69</v>
       </c>
-      <c r="G40" s="68">
+      <c r="G40" s="65">
         <v>0.68</v>
       </c>
-      <c r="H40" s="68">
+      <c r="H40" s="65">
         <v>0.67</v>
       </c>
-      <c r="I40" s="68">
+      <c r="I40" s="65">
         <v>0.66</v>
       </c>
-      <c r="J40" s="68">
+      <c r="J40" s="65">
         <v>0.65</v>
       </c>
-      <c r="K40" s="68">
+      <c r="K40" s="65">
         <v>0.64</v>
       </c>
-      <c r="L40" s="68">
+      <c r="L40" s="65">
         <v>0.63</v>
       </c>
-      <c r="M40" s="68">
+      <c r="M40" s="65">
         <v>0.62</v>
       </c>
-      <c r="N40" s="68">
+      <c r="N40" s="65">
         <v>0.61</v>
       </c>
-      <c r="O40" s="68">
+      <c r="O40" s="65">
         <v>0.6</v>
       </c>
-      <c r="P40" s="68">
+      <c r="P40" s="65">
         <v>0.59</v>
       </c>
-      <c r="Q40" s="68">
+      <c r="Q40" s="65">
         <v>0.57999999999999996</v>
       </c>
-      <c r="R40" s="68">
+      <c r="R40" s="65">
         <v>0.56999999999999995</v>
       </c>
-      <c r="S40" s="68">
+      <c r="S40" s="65">
         <v>0.56000000000000005</v>
       </c>
       <c r="T40" s="11" t="s">
@@ -16292,164 +16432,164 @@
       <c r="U40" s="14"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B41" s="62" t="s">
+      <c r="B41" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="68">
+      <c r="C41" s="65">
         <v>0.7</v>
       </c>
-      <c r="D41" s="68">
+      <c r="D41" s="65">
         <v>0.71</v>
       </c>
-      <c r="E41" s="68">
+      <c r="E41" s="65">
         <v>0.72</v>
       </c>
-      <c r="F41" s="68">
+      <c r="F41" s="65">
         <v>0.73</v>
       </c>
-      <c r="G41" s="68">
+      <c r="G41" s="65">
         <v>0.74</v>
       </c>
-      <c r="H41" s="68">
+      <c r="H41" s="65">
         <v>0.75</v>
       </c>
-      <c r="I41" s="68">
+      <c r="I41" s="65">
         <v>0.76</v>
       </c>
-      <c r="J41" s="68">
+      <c r="J41" s="65">
         <v>0.77</v>
       </c>
-      <c r="K41" s="68">
+      <c r="K41" s="65">
         <v>0.78</v>
       </c>
-      <c r="L41" s="68">
+      <c r="L41" s="65">
         <v>0.79</v>
       </c>
-      <c r="M41" s="68">
+      <c r="M41" s="65">
         <v>0.8</v>
       </c>
-      <c r="N41" s="68">
+      <c r="N41" s="65">
         <v>0.81</v>
       </c>
-      <c r="O41" s="68">
+      <c r="O41" s="65">
         <v>0.82</v>
       </c>
-      <c r="P41" s="68">
+      <c r="P41" s="65">
         <v>0.83</v>
       </c>
-      <c r="Q41" s="68">
+      <c r="Q41" s="65">
         <v>0.84</v>
       </c>
-      <c r="R41" s="68">
+      <c r="R41" s="65">
         <v>0.85</v>
       </c>
-      <c r="S41" s="68">
+      <c r="S41" s="65">
         <v>0.86</v>
       </c>
       <c r="T41" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U41" s="65"/>
+      <c r="U41" s="62"/>
     </row>
     <row r="42" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="70"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="70"/>
-      <c r="M42" s="70"/>
-      <c r="N42" s="70"/>
-      <c r="O42" s="70"/>
-      <c r="P42" s="70"/>
-      <c r="Q42" s="70"/>
-      <c r="R42" s="70"/>
-      <c r="S42" s="70"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="67"/>
+      <c r="P42" s="67"/>
+      <c r="Q42" s="67"/>
+      <c r="R42" s="67"/>
+      <c r="S42" s="67"/>
       <c r="T42" s="19"/>
-      <c r="U42" s="63"/>
+      <c r="U42" s="60"/>
     </row>
     <row r="43" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="66"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="70"/>
-      <c r="K43" s="70"/>
-      <c r="L43" s="70"/>
-      <c r="M43" s="70"/>
-      <c r="N43" s="70"/>
-      <c r="O43" s="70"/>
-      <c r="P43" s="70"/>
-      <c r="Q43" s="70"/>
-      <c r="R43" s="70"/>
-      <c r="S43" s="70"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="67"/>
+      <c r="O43" s="67"/>
+      <c r="P43" s="67"/>
+      <c r="Q43" s="67"/>
+      <c r="R43" s="67"/>
+      <c r="S43" s="67"/>
       <c r="T43" s="19"/>
-      <c r="U43" s="63"/>
+      <c r="U43" s="60"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B44" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="68">
+      <c r="C44" s="65">
         <v>0.35</v>
       </c>
-      <c r="D44" s="68">
+      <c r="D44" s="65">
         <v>0.34</v>
       </c>
-      <c r="E44" s="68">
+      <c r="E44" s="65">
         <v>0.33</v>
       </c>
-      <c r="F44" s="68">
+      <c r="F44" s="65">
         <v>0.32</v>
       </c>
-      <c r="G44" s="68">
+      <c r="G44" s="65">
         <v>0.31</v>
       </c>
-      <c r="H44" s="68">
+      <c r="H44" s="65">
         <v>0.3</v>
       </c>
-      <c r="I44" s="68">
+      <c r="I44" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J44" s="68">
+      <c r="J44" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K44" s="68">
+      <c r="K44" s="65">
         <v>0.27</v>
       </c>
-      <c r="L44" s="68">
+      <c r="L44" s="65">
         <v>0.26</v>
       </c>
-      <c r="M44" s="68">
+      <c r="M44" s="65">
         <v>0.25</v>
       </c>
-      <c r="N44" s="68">
+      <c r="N44" s="65">
         <v>0.24000000000000099</v>
       </c>
-      <c r="O44" s="68">
+      <c r="O44" s="65">
         <v>0.23000000000000101</v>
       </c>
-      <c r="P44" s="68">
+      <c r="P44" s="65">
         <v>0.220000000000001</v>
       </c>
-      <c r="Q44" s="68">
+      <c r="Q44" s="65">
         <v>0.21000000000000099</v>
       </c>
-      <c r="R44" s="68">
+      <c r="R44" s="65">
         <v>0.20000000000000101</v>
       </c>
-      <c r="S44" s="68">
+      <c r="S44" s="65">
         <v>0.190000000000001</v>
       </c>
       <c r="T44" s="11" t="s">
@@ -16461,55 +16601,55 @@
       <c r="B45" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="68">
+      <c r="C45" s="65">
         <v>0.34</v>
       </c>
-      <c r="D45" s="68">
+      <c r="D45" s="65">
         <v>0.33</v>
       </c>
-      <c r="E45" s="68">
+      <c r="E45" s="65">
         <v>0.32</v>
       </c>
-      <c r="F45" s="68">
+      <c r="F45" s="65">
         <v>0.31</v>
       </c>
-      <c r="G45" s="68">
+      <c r="G45" s="65">
         <v>0.3</v>
       </c>
-      <c r="H45" s="68">
+      <c r="H45" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I45" s="68">
+      <c r="I45" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J45" s="68">
+      <c r="J45" s="65">
         <v>0.27</v>
       </c>
-      <c r="K45" s="68">
+      <c r="K45" s="65">
         <v>0.26</v>
       </c>
-      <c r="L45" s="68">
+      <c r="L45" s="65">
         <v>0.25</v>
       </c>
-      <c r="M45" s="68">
+      <c r="M45" s="65">
         <v>0.24</v>
       </c>
-      <c r="N45" s="68">
+      <c r="N45" s="65">
         <v>0.23</v>
       </c>
-      <c r="O45" s="68">
+      <c r="O45" s="65">
         <v>0.22</v>
       </c>
-      <c r="P45" s="68">
+      <c r="P45" s="65">
         <v>0.21</v>
       </c>
-      <c r="Q45" s="68">
+      <c r="Q45" s="65">
         <v>0.2</v>
       </c>
-      <c r="R45" s="68">
+      <c r="R45" s="65">
         <v>0.19</v>
       </c>
-      <c r="S45" s="68">
+      <c r="S45" s="65">
         <v>0.18</v>
       </c>
       <c r="T45" s="11" t="s">
@@ -16521,55 +16661,55 @@
       <c r="B46" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="68">
+      <c r="C46" s="65">
         <v>0.32</v>
       </c>
-      <c r="D46" s="68">
+      <c r="D46" s="65">
         <v>0.31</v>
       </c>
-      <c r="E46" s="68">
+      <c r="E46" s="65">
         <v>0.3</v>
       </c>
-      <c r="F46" s="68">
+      <c r="F46" s="65">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G46" s="68">
+      <c r="G46" s="65">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H46" s="68">
+      <c r="H46" s="65">
         <v>0.27</v>
       </c>
-      <c r="I46" s="68">
+      <c r="I46" s="65">
         <v>0.26</v>
       </c>
-      <c r="J46" s="68">
+      <c r="J46" s="65">
         <v>0.25</v>
       </c>
-      <c r="K46" s="68">
+      <c r="K46" s="65">
         <v>0.24</v>
       </c>
-      <c r="L46" s="68">
+      <c r="L46" s="65">
         <v>0.23</v>
       </c>
-      <c r="M46" s="68">
+      <c r="M46" s="65">
         <v>0.22</v>
       </c>
-      <c r="N46" s="68">
+      <c r="N46" s="65">
         <v>0.21</v>
       </c>
-      <c r="O46" s="68">
+      <c r="O46" s="65">
         <v>0.2</v>
       </c>
-      <c r="P46" s="68">
+      <c r="P46" s="65">
         <v>0.19</v>
       </c>
-      <c r="Q46" s="68">
+      <c r="Q46" s="65">
         <v>0.18</v>
       </c>
-      <c r="R46" s="68">
+      <c r="R46" s="65">
         <v>0.17</v>
       </c>
-      <c r="S46" s="68">
+      <c r="S46" s="65">
         <v>0.16</v>
       </c>
       <c r="T46" s="11" t="s">
@@ -16578,104 +16718,104 @@
       <c r="U46" s="14"/>
     </row>
     <row r="47" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="70"/>
-      <c r="N47" s="70"/>
-      <c r="O47" s="70"/>
-      <c r="P47" s="70"/>
-      <c r="Q47" s="70"/>
-      <c r="R47" s="70"/>
-      <c r="S47" s="70"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="67"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="67"/>
+      <c r="M47" s="67"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="67"/>
+      <c r="P47" s="67"/>
+      <c r="Q47" s="67"/>
+      <c r="R47" s="67"/>
+      <c r="S47" s="67"/>
       <c r="T47" s="19"/>
-      <c r="U47" s="63"/>
+      <c r="U47" s="60"/>
     </row>
     <row r="48" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="66"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="70"/>
-      <c r="H48" s="70"/>
-      <c r="I48" s="70"/>
-      <c r="J48" s="70"/>
-      <c r="K48" s="70"/>
-      <c r="L48" s="70"/>
-      <c r="M48" s="70"/>
-      <c r="N48" s="70"/>
-      <c r="O48" s="70"/>
-      <c r="P48" s="70"/>
-      <c r="Q48" s="70"/>
-      <c r="R48" s="70"/>
-      <c r="S48" s="70"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="67"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="67"/>
+      <c r="M48" s="67"/>
+      <c r="N48" s="67"/>
+      <c r="O48" s="67"/>
+      <c r="P48" s="67"/>
+      <c r="Q48" s="67"/>
+      <c r="R48" s="67"/>
+      <c r="S48" s="67"/>
       <c r="T48" s="19"/>
-      <c r="U48" s="63"/>
+      <c r="U48" s="60"/>
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="68">
+      <c r="C49" s="65">
         <v>0.27</v>
       </c>
-      <c r="D49" s="68">
+      <c r="D49" s="65">
         <v>0.26</v>
       </c>
-      <c r="E49" s="68">
+      <c r="E49" s="65">
         <v>0.25</v>
       </c>
-      <c r="F49" s="68">
+      <c r="F49" s="65">
         <v>0.24</v>
       </c>
-      <c r="G49" s="68">
+      <c r="G49" s="65">
         <v>0.23</v>
       </c>
-      <c r="H49" s="68">
+      <c r="H49" s="65">
         <v>0.22</v>
       </c>
-      <c r="I49" s="68">
+      <c r="I49" s="65">
         <v>0.21</v>
       </c>
-      <c r="J49" s="68">
+      <c r="J49" s="65">
         <v>0.2</v>
       </c>
-      <c r="K49" s="68">
+      <c r="K49" s="65">
         <v>0.19</v>
       </c>
-      <c r="L49" s="68">
+      <c r="L49" s="65">
         <v>0.18</v>
       </c>
-      <c r="M49" s="68">
+      <c r="M49" s="65">
         <v>0.17</v>
       </c>
-      <c r="N49" s="68">
+      <c r="N49" s="65">
         <v>0.16</v>
       </c>
-      <c r="O49" s="68">
+      <c r="O49" s="65">
         <v>0.15</v>
       </c>
-      <c r="P49" s="68">
+      <c r="P49" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="Q49" s="68">
+      <c r="Q49" s="65">
         <v>0.13</v>
       </c>
-      <c r="R49" s="68">
+      <c r="R49" s="65">
         <v>0.12</v>
       </c>
-      <c r="S49" s="68">
+      <c r="S49" s="65">
         <v>0.11</v>
       </c>
       <c r="T49" s="11" t="s">
@@ -16687,55 +16827,55 @@
       <c r="B50" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="68">
+      <c r="C50" s="65">
         <v>0.25</v>
       </c>
-      <c r="D50" s="68">
+      <c r="D50" s="65">
         <v>0.24</v>
       </c>
-      <c r="E50" s="68">
+      <c r="E50" s="65">
         <v>0.23</v>
       </c>
-      <c r="F50" s="68">
+      <c r="F50" s="65">
         <v>0.22</v>
       </c>
-      <c r="G50" s="68">
+      <c r="G50" s="65">
         <v>0.21</v>
       </c>
-      <c r="H50" s="68">
+      <c r="H50" s="65">
         <v>0.2</v>
       </c>
-      <c r="I50" s="68">
+      <c r="I50" s="65">
         <v>0.19</v>
       </c>
-      <c r="J50" s="68">
+      <c r="J50" s="65">
         <v>0.18</v>
       </c>
-      <c r="K50" s="68">
+      <c r="K50" s="65">
         <v>0.17</v>
       </c>
-      <c r="L50" s="68">
+      <c r="L50" s="65">
         <v>0.16</v>
       </c>
-      <c r="M50" s="68">
+      <c r="M50" s="65">
         <v>0.15</v>
       </c>
-      <c r="N50" s="68">
+      <c r="N50" s="65">
         <v>0.14000000000000001</v>
       </c>
-      <c r="O50" s="68">
+      <c r="O50" s="65">
         <v>0.13</v>
       </c>
-      <c r="P50" s="68">
+      <c r="P50" s="65">
         <v>0.12</v>
       </c>
-      <c r="Q50" s="68">
+      <c r="Q50" s="65">
         <v>0.11</v>
       </c>
-      <c r="R50" s="68">
+      <c r="R50" s="65">
         <v>0.1</v>
       </c>
-      <c r="S50" s="68">
+      <c r="S50" s="65">
         <v>0.09</v>
       </c>
       <c r="T50" s="11" t="s">
@@ -16747,55 +16887,55 @@
       <c r="B51" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="68">
+      <c r="C51" s="65">
         <v>0.23</v>
       </c>
-      <c r="D51" s="68">
+      <c r="D51" s="65">
         <v>0.21</v>
       </c>
-      <c r="E51" s="68">
+      <c r="E51" s="65">
         <v>0.19</v>
       </c>
-      <c r="F51" s="68">
+      <c r="F51" s="65">
         <v>0.17</v>
       </c>
-      <c r="G51" s="68">
+      <c r="G51" s="65">
         <v>0.15</v>
       </c>
-      <c r="H51" s="68">
+      <c r="H51" s="65">
         <v>0.13</v>
       </c>
-      <c r="I51" s="68">
+      <c r="I51" s="65">
         <v>0.11</v>
       </c>
-      <c r="J51" s="68">
+      <c r="J51" s="65">
         <v>0.09</v>
       </c>
-      <c r="K51" s="68">
+      <c r="K51" s="65">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L51" s="68">
+      <c r="L51" s="65">
         <v>0.05</v>
       </c>
-      <c r="M51" s="68">
+      <c r="M51" s="65">
         <v>0.03</v>
       </c>
-      <c r="N51" s="68">
+      <c r="N51" s="65">
         <v>0.01</v>
       </c>
-      <c r="O51" s="68">
+      <c r="O51" s="65">
         <v>-9.9999999999999794E-3</v>
       </c>
-      <c r="P51" s="68">
+      <c r="P51" s="65">
         <v>-0.03</v>
       </c>
-      <c r="Q51" s="68">
+      <c r="Q51" s="65">
         <v>-0.05</v>
       </c>
-      <c r="R51" s="68">
+      <c r="R51" s="65">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="S51" s="68">
+      <c r="S51" s="65">
         <v>-0.09</v>
       </c>
       <c r="T51" s="11" t="s">
@@ -16822,7 +16962,7 @@
       <c r="R52" s="18"/>
       <c r="S52" s="18"/>
       <c r="T52" s="19"/>
-      <c r="U52" s="63"/>
+      <c r="U52" s="60"/>
     </row>
     <row r="53" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="18"/>
@@ -16843,7 +16983,7 @@
       <c r="R53" s="18"/>
       <c r="S53" s="18"/>
       <c r="T53" s="19"/>
-      <c r="U53" s="63"/>
+      <c r="U53" s="60"/>
     </row>
     <row r="54" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="18"/>
@@ -16864,7 +17004,7 @@
       <c r="R54" s="18"/>
       <c r="S54" s="18"/>
       <c r="T54" s="19"/>
-      <c r="U54" s="63"/>
+      <c r="U54" s="60"/>
     </row>
     <row r="55" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="18"/>
@@ -16885,7 +17025,7 @@
       <c r="R55" s="18"/>
       <c r="S55" s="18"/>
       <c r="T55" s="19"/>
-      <c r="U55" s="63"/>
+      <c r="U55" s="60"/>
     </row>
     <row r="56" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="18"/>
@@ -16906,7 +17046,7 @@
       <c r="R56" s="18"/>
       <c r="S56" s="18"/>
       <c r="T56" s="19"/>
-      <c r="U56" s="63"/>
+      <c r="U56" s="60"/>
     </row>
     <row r="57" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="18"/>
@@ -16927,7 +17067,7 @@
       <c r="R57" s="18"/>
       <c r="S57" s="18"/>
       <c r="T57" s="19"/>
-      <c r="U57" s="63"/>
+      <c r="U57" s="60"/>
     </row>
     <row r="58" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="18"/>
@@ -16948,7 +17088,7 @@
       <c r="R58" s="18"/>
       <c r="S58" s="18"/>
       <c r="T58" s="19"/>
-      <c r="U58" s="63"/>
+      <c r="U58" s="60"/>
     </row>
     <row r="59" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="18"/>
@@ -16969,7 +17109,7 @@
       <c r="R59" s="18"/>
       <c r="S59" s="18"/>
       <c r="T59" s="19"/>
-      <c r="U59" s="63"/>
+      <c r="U59" s="60"/>
     </row>
     <row r="60" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="18"/>
@@ -16990,7 +17130,7 @@
       <c r="R60" s="18"/>
       <c r="S60" s="18"/>
       <c r="T60" s="19"/>
-      <c r="U60" s="63"/>
+      <c r="U60" s="60"/>
     </row>
     <row r="61" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="18"/>
@@ -17011,7 +17151,7 @@
       <c r="R61" s="18"/>
       <c r="S61" s="18"/>
       <c r="T61" s="19"/>
-      <c r="U61" s="63"/>
+      <c r="U61" s="60"/>
     </row>
     <row r="62" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="18"/>
@@ -17032,7 +17172,7 @@
       <c r="R62" s="18"/>
       <c r="S62" s="18"/>
       <c r="T62" s="19"/>
-      <c r="U62" s="63"/>
+      <c r="U62" s="60"/>
     </row>
     <row r="63" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="18"/>
@@ -17053,7 +17193,7 @@
       <c r="R63" s="18"/>
       <c r="S63" s="18"/>
       <c r="T63" s="19"/>
-      <c r="U63" s="63"/>
+      <c r="U63" s="60"/>
     </row>
     <row r="64" spans="2:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="18"/>
@@ -17074,7 +17214,7 @@
       <c r="R64" s="18"/>
       <c r="S64" s="18"/>
       <c r="T64" s="19"/>
-      <c r="U64" s="63"/>
+      <c r="U64" s="60"/>
     </row>
     <row r="65" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="18"/>
@@ -17095,7 +17235,7 @@
       <c r="R65" s="18"/>
       <c r="S65" s="18"/>
       <c r="T65" s="19"/>
-      <c r="U65" s="63"/>
+      <c r="U65" s="60"/>
     </row>
     <row r="66" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="18"/>
@@ -17116,7 +17256,7 @@
       <c r="R66" s="18"/>
       <c r="S66" s="18"/>
       <c r="T66" s="19"/>
-      <c r="U66" s="63"/>
+      <c r="U66" s="60"/>
     </row>
     <row r="67" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="18"/>
@@ -17137,7 +17277,7 @@
       <c r="R67" s="18"/>
       <c r="S67" s="18"/>
       <c r="T67" s="19"/>
-      <c r="U67" s="63"/>
+      <c r="U67" s="60"/>
     </row>
     <row r="68" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C68" s="18"/>
@@ -17158,7 +17298,7 @@
       <c r="R68" s="18"/>
       <c r="S68" s="18"/>
       <c r="T68" s="19"/>
-      <c r="U68" s="63"/>
+      <c r="U68" s="60"/>
     </row>
     <row r="69" spans="3:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C69" s="18"/>
@@ -17179,7 +17319,7 @@
       <c r="R69" s="18"/>
       <c r="S69" s="18"/>
       <c r="T69" s="19"/>
-      <c r="U69" s="63"/>
+      <c r="U69" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>